<commit_message>
updates vocab metadata for publish date, etc.
- changes the publish date for all vocabs to 31 MAY 2024 for v2
- changes the templates for all HTML docs to be consistent
- HTML title, publish date, version is taken from RDF metadata
- added funding acknowledgements to all pages
- scripts for generating UCR, examples, primer
- closes #149 by adding key publications to each page
- updates editor's draft URI to dev.dpvcg.org
</commit_message>
<xml_diff>
--- a/code/vocab_csv/tech.xlsx
+++ b/code/vocab_csv/tech.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1298" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1295" uniqueCount="518">
   <si>
     <t>Term</t>
   </si>
@@ -11078,9 +11078,7 @@
       <c r="F2" s="6" t="s">
         <v>422</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
@@ -11130,9 +11128,7 @@
       <c r="F3" s="6" t="s">
         <v>422</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
@@ -11178,9 +11174,7 @@
       <c r="F4" s="6" t="s">
         <v>422</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>

</xml_diff>

<commit_message>
tech: fix missing TechnologyStatus concept
- added concept to spreadsheet and extension
- added missing label for MarketAvailabilityStatus
</commit_message>
<xml_diff>
--- a/code/vocab_csv/tech.xlsx
+++ b/code/vocab_csv/tech.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1295" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1302" uniqueCount="523">
   <si>
     <t>Term</t>
   </si>
@@ -1215,10 +1215,25 @@
     <t>DeploymentStatus</t>
   </si>
   <si>
+    <t>TechnologyStatus</t>
+  </si>
+  <si>
+    <t>Technology Status</t>
+  </si>
+  <si>
+    <t>Status associated with development, deployment, and use of technology</t>
+  </si>
+  <si>
     <t>MarketAvailabilityStatus</t>
   </si>
   <si>
+    <t>Market Availability Status</t>
+  </si>
+  <si>
     <t>Status indicating whether Technology is available on the market</t>
+  </si>
+  <si>
+    <t>tech:TechnologyStatus</t>
   </si>
   <si>
     <t>MarketAvailable</t>
@@ -2809,10 +2824,10 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>429</v>
+        <v>434</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>429</v>
+        <v>434</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -2827,13 +2842,13 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>430</v>
+        <v>435</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>430</v>
+        <v>435</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>431</v>
+        <v>436</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="22" t="s">
@@ -2873,16 +2888,16 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>432</v>
+        <v>437</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>433</v>
+        <v>438</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>434</v>
+        <v>439</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>435</v>
+        <v>440</v>
       </c>
       <c r="E5" s="22" t="s">
         <v>60</v>
@@ -2921,16 +2936,16 @@
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>436</v>
+        <v>441</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>436</v>
+        <v>441</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>437</v>
+        <v>442</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>435</v>
+        <v>440</v>
       </c>
       <c r="E6" s="22" t="s">
         <v>60</v>
@@ -2969,16 +2984,16 @@
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>438</v>
+        <v>443</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>438</v>
+        <v>443</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>439</v>
+        <v>444</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>435</v>
+        <v>440</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>60</v>
@@ -3017,16 +3032,16 @@
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>440</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>440</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>441</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>435</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>60</v>
@@ -3065,16 +3080,16 @@
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>442</v>
+        <v>447</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>444</v>
+        <v>449</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>435</v>
+        <v>440</v>
       </c>
       <c r="E9" s="22" t="s">
         <v>60</v>
@@ -3113,13 +3128,13 @@
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
-        <v>445</v>
+        <v>450</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>445</v>
+        <v>450</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>446</v>
+        <v>451</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="22" t="s">
@@ -3257,10 +3272,10 @@
     </row>
     <row r="2">
       <c r="A2" s="38" t="s">
-        <v>447</v>
+        <v>452</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>447</v>
+        <v>452</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="39"/>
@@ -3279,13 +3294,13 @@
     </row>
     <row r="4">
       <c r="A4" s="38" t="s">
-        <v>448</v>
+        <v>453</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>448</v>
+        <v>453</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>449</v>
+        <v>454</v>
       </c>
       <c r="D4" s="40"/>
       <c r="E4" s="6" t="s">
@@ -3331,16 +3346,16 @@
     </row>
     <row r="6">
       <c r="A6" s="38" t="s">
-        <v>450</v>
+        <v>455</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>451</v>
+        <v>456</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>453</v>
+        <v>458</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>16</v>
@@ -3375,16 +3390,16 @@
     </row>
     <row r="7">
       <c r="A7" s="24" t="s">
-        <v>454</v>
+        <v>459</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>454</v>
+        <v>459</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>455</v>
+        <v>460</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>456</v>
+        <v>461</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>16</v>
@@ -3425,16 +3440,16 @@
     </row>
     <row r="8">
       <c r="A8" s="17" t="s">
-        <v>457</v>
+        <v>462</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>458</v>
+        <v>463</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>459</v>
+        <v>464</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>456</v>
+        <v>461</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>16</v>
@@ -3469,16 +3484,16 @@
     </row>
     <row r="9">
       <c r="A9" s="17" t="s">
-        <v>460</v>
+        <v>465</v>
       </c>
       <c r="B9" s="17" t="s">
+        <v>466</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>467</v>
+      </c>
+      <c r="D9" s="25" t="s">
         <v>461</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>462</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>456</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>16</v>
@@ -3513,16 +3528,16 @@
     </row>
     <row r="10">
       <c r="A10" s="24" t="s">
-        <v>463</v>
+        <v>468</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>463</v>
+        <v>468</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>464</v>
+        <v>469</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>465</v>
+        <v>470</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>16</v>
@@ -3569,10 +3584,10 @@
         <v>158</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>453</v>
+        <v>458</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>16</v>
@@ -3607,16 +3622,16 @@
     </row>
     <row r="13">
       <c r="A13" s="24" t="s">
-        <v>467</v>
+        <v>472</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>468</v>
+        <v>473</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>469</v>
+        <v>474</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>16</v>
@@ -3657,16 +3672,16 @@
     </row>
     <row r="14">
       <c r="A14" s="6" t="s">
-        <v>471</v>
+        <v>476</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>472</v>
+        <v>477</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>473</v>
+        <v>478</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>16</v>
@@ -3701,16 +3716,16 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>474</v>
+        <v>479</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>475</v>
+        <v>480</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>476</v>
+        <v>481</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>453</v>
+        <v>458</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>16</v>
@@ -3745,16 +3760,16 @@
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>478</v>
+        <v>483</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>479</v>
+        <v>484</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>480</v>
+        <v>485</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>16</v>
@@ -3789,16 +3804,16 @@
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>480</v>
+        <v>485</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>16</v>
@@ -3833,16 +3848,16 @@
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>484</v>
+        <v>489</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>480</v>
+        <v>485</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>16</v>
@@ -3877,16 +3892,16 @@
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>491</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>492</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>485</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>486</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>487</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>480</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>16</v>
@@ -3921,13 +3936,13 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>488</v>
+        <v>493</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>488</v>
+        <v>493</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>489</v>
+        <v>494</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="6" t="s">
@@ -3966,16 +3981,16 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>490</v>
+        <v>495</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>490</v>
+        <v>495</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>491</v>
+        <v>496</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>492</v>
+        <v>497</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>16</v>
@@ -4010,16 +4025,16 @@
     </row>
     <row r="25">
       <c r="A25" s="6" t="s">
-        <v>493</v>
+        <v>498</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>494</v>
+        <v>499</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>495</v>
+        <v>500</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>496</v>
+        <v>501</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>16</v>
@@ -4054,16 +4069,16 @@
     </row>
     <row r="26">
       <c r="A26" s="6" t="s">
-        <v>497</v>
+        <v>502</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>498</v>
+        <v>503</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>499</v>
+        <v>504</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>500</v>
+        <v>505</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>16</v>
@@ -4098,16 +4113,16 @@
     </row>
     <row r="27">
       <c r="A27" s="6" t="s">
-        <v>501</v>
+        <v>506</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>502</v>
+        <v>507</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>503</v>
+        <v>508</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>500</v>
+        <v>505</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>16</v>
@@ -4142,16 +4157,16 @@
     </row>
     <row r="28">
       <c r="A28" s="6" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>496</v>
+        <v>501</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>16</v>
@@ -4186,16 +4201,16 @@
     </row>
     <row r="29">
       <c r="A29" s="6" t="s">
-        <v>505</v>
+        <v>510</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>506</v>
+        <v>511</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>507</v>
+        <v>512</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>508</v>
+        <v>513</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>16</v>
@@ -4230,16 +4245,16 @@
     </row>
     <row r="30">
       <c r="A30" s="6" t="s">
-        <v>509</v>
+        <v>514</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>509</v>
+        <v>514</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>510</v>
+        <v>515</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>511</v>
+        <v>516</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>16</v>
@@ -4375,27 +4390,27 @@
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>512</v>
+        <v>517</v>
       </c>
       <c r="B2" s="5"/>
       <c r="J2" s="10" t="s">
-        <v>513</v>
+        <v>518</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>514</v>
+        <v>519</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>517</v>
+        <v>522</v>
       </c>
     </row>
     <row r="6">
@@ -10625,9 +10640,11 @@
       <c r="A6" s="17" t="s">
         <v>397</v>
       </c>
-      <c r="B6" s="17"/>
+      <c r="B6" s="17" t="s">
+        <v>398</v>
+      </c>
       <c r="C6" s="17" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>394</v>
@@ -10641,16 +10658,14 @@
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="8">
-        <v>45421.0</v>
+        <v>45443.0</v>
       </c>
       <c r="L6" s="7"/>
       <c r="M6" s="6" t="s">
         <v>26</v>
       </c>
       <c r="N6" s="7"/>
-      <c r="O6" s="9" t="s">
-        <v>28</v>
-      </c>
+      <c r="O6" s="6"/>
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
@@ -10670,17 +10685,19 @@
     </row>
     <row r="7">
       <c r="A7" s="17" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>401</v>
-      </c>
-      <c r="D7" s="7"/>
+        <v>402</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>403</v>
+      </c>
       <c r="E7" s="6" t="s">
-        <v>402</v>
+        <v>25</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -10695,7 +10712,9 @@
         <v>26</v>
       </c>
       <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
+      <c r="O7" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
       <c r="R7" s="7"/>
@@ -10715,17 +10734,17 @@
     </row>
     <row r="8">
       <c r="A8" s="17" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="6" t="s">
-        <v>402</v>
+        <v>407</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
@@ -10759,26 +10778,24 @@
       <c r="AE8" s="7"/>
     </row>
     <row r="9">
-      <c r="A9" s="32" t="s">
-        <v>406</v>
-      </c>
-      <c r="B9" s="32" t="s">
+      <c r="A9" s="17" t="s">
+        <v>408</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>409</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>410</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="6" t="s">
         <v>407</v>
       </c>
-      <c r="C9" s="32" t="s">
-        <v>408</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>394</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="32"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
       <c r="K9" s="8">
         <v>45421.0</v>
       </c>
@@ -10786,44 +10803,46 @@
       <c r="M9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="N9" s="21"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="21"/>
-      <c r="S9" s="21"/>
-      <c r="T9" s="21"/>
-      <c r="U9" s="21"/>
-      <c r="V9" s="21"/>
-      <c r="W9" s="21"/>
-      <c r="X9" s="21"/>
-      <c r="Y9" s="21"/>
-      <c r="Z9" s="21"/>
-      <c r="AA9" s="21"/>
-      <c r="AB9" s="21"/>
-      <c r="AC9" s="21"/>
-      <c r="AD9" s="21"/>
-      <c r="AE9" s="21"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="7"/>
+      <c r="AA9" s="7"/>
+      <c r="AB9" s="7"/>
+      <c r="AC9" s="7"/>
+      <c r="AD9" s="7"/>
+      <c r="AE9" s="7"/>
     </row>
     <row r="10">
       <c r="A10" s="32" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>410</v>
-      </c>
-      <c r="D10" s="7"/>
+        <v>413</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>403</v>
+      </c>
       <c r="E10" s="6" t="s">
-        <v>411</v>
+        <v>25</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
+      <c r="J10" s="32"/>
       <c r="K10" s="8">
         <v>45421.0</v>
       </c>
@@ -10852,17 +10871,17 @@
     </row>
     <row r="11">
       <c r="A11" s="32" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>413</v>
-      </c>
-      <c r="C11" s="22" t="s">
         <v>414</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>415</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="6" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
@@ -10896,26 +10915,24 @@
       <c r="AE11" s="21"/>
     </row>
     <row r="12">
-      <c r="A12" s="6" t="s">
-        <v>415</v>
-      </c>
-      <c r="B12" s="6" t="s">
+      <c r="A12" s="32" t="s">
+        <v>417</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>418</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>419</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="6" t="s">
         <v>416</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>417</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
       <c r="K12" s="8">
         <v>45421.0</v>
       </c>
@@ -10923,74 +10940,121 @@
       <c r="M12" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="N12" s="6" t="s">
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="21"/>
+      <c r="T12" s="21"/>
+      <c r="U12" s="21"/>
+      <c r="V12" s="21"/>
+      <c r="W12" s="21"/>
+      <c r="X12" s="21"/>
+      <c r="Y12" s="21"/>
+      <c r="Z12" s="21"/>
+      <c r="AA12" s="21"/>
+      <c r="AB12" s="21"/>
+      <c r="AC12" s="21"/>
+      <c r="AD12" s="21"/>
+      <c r="AE12" s="21"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="s">
+        <v>420</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="8">
+        <v>45421.0</v>
+      </c>
+      <c r="L13" s="7"/>
+      <c r="M13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="N13" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="O12" s="9" t="s">
+      <c r="O13" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
-      <c r="T12" s="7"/>
-      <c r="U12" s="7"/>
-      <c r="V12" s="7"/>
-      <c r="W12" s="7"/>
-      <c r="X12" s="7"/>
-      <c r="Y12" s="7"/>
-      <c r="Z12" s="7"/>
-      <c r="AA12" s="7"/>
-      <c r="AB12" s="7"/>
-      <c r="AC12" s="7"/>
-      <c r="AD12" s="7"/>
-      <c r="AE12" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+      <c r="V13" s="7"/>
+      <c r="W13" s="7"/>
+      <c r="X13" s="7"/>
+      <c r="Y13" s="7"/>
+      <c r="Z13" s="7"/>
+      <c r="AA13" s="7"/>
+      <c r="AB13" s="7"/>
+      <c r="AC13" s="7"/>
+      <c r="AD13" s="7"/>
+      <c r="AE13" s="7"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A12:AD12">
+  <conditionalFormatting sqref="A13:AD13">
     <cfRule type="expression" dxfId="3" priority="1">
-      <formula>$M12="deprecated"</formula>
+      <formula>$M13="deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A12:AD12">
+  <conditionalFormatting sqref="A13:AD13">
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>$M12="accepted"</formula>
+      <formula>$M13="accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A12:AB12">
+  <conditionalFormatting sqref="A13:AB13">
     <cfRule type="expression" dxfId="1" priority="3">
-      <formula>$M12="proposed"</formula>
+      <formula>$M13="proposed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A12:AB12">
+  <conditionalFormatting sqref="A13:AB13">
     <cfRule type="expression" dxfId="2" priority="4">
-      <formula>$M12="changed"</formula>
+      <formula>$M13="changed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:J11 K2:M140 N2:AD11 AE2:AE140 A13:J140 N13:AD140">
+  <conditionalFormatting sqref="A2:J12 K2:M141 N2:AD12 AE2:AE141 A14:J141 N14:AD141">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>$M2="accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:J11 K2:M116 N2:AB11 A13:J116 N13:AB116">
+  <conditionalFormatting sqref="A2:J12 K2:M117 N2:AB12 A14:J117 N14:AB117">
     <cfRule type="expression" dxfId="1" priority="6">
       <formula>$M2="proposed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:J11 K2:M116 N2:AB11 A13:J116 N13:AB116">
+  <conditionalFormatting sqref="A2:J12 K2:M117 N2:AB12 A14:J117 N14:AB117">
     <cfRule type="expression" dxfId="2" priority="7">
       <formula>$M2="changed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2 M2:M140 N2:O11 J4:J11 K7:K11 A9:I11 L9:L11 P9:AD11 AE9:AE140 A13:L140 N13:AD140">
+  <conditionalFormatting sqref="K2 M2:M141 N2:O12 J4:J12 K8:K12 A10:I12 L10:L12 P10:AD12 AE10:AE141 A14:L141 N14:AD141">
     <cfRule type="expression" dxfId="3" priority="8">
       <formula>$M2="deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="O4"/>
-    <hyperlink r:id="rId2" ref="O6"/>
-    <hyperlink r:id="rId3" ref="O12"/>
+    <hyperlink r:id="rId2" ref="O7"/>
+    <hyperlink r:id="rId3" ref="O13"/>
   </hyperlinks>
   <drawing r:id="rId4"/>
 </worksheet>
@@ -11061,22 +11125,22 @@
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>419</v>
+        <v>424</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>420</v>
+        <v>425</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>421</v>
+        <v>426</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -11111,22 +11175,22 @@
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>423</v>
+        <v>428</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>424</v>
+        <v>429</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>425</v>
+        <v>430</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>402</v>
+        <v>407</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -11157,22 +11221,22 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>426</v>
+        <v>431</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>427</v>
+        <v>432</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>428</v>
+        <v>433</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>

</xml_diff>

<commit_message>
minor fixes, reference updates
- changed range (includes) of DPV entity properties to dpv:Entity
  instead of dpv:EntityInvolvement - dpv:hasActiveEntity,
  dpv:hasPassiveEntity, and dpv:hasNonInvolvedEntity
- added property tech:hasDocumentation which was missing and is needed
  to link to tech:Documentation concepts
- fixed examples E000, E0043 for contents, and replaced non-ASCII
  quotation marks in examples where they occured
- updated reference to DCAT which was titled with "DCAT v2" whereas we
  now have DCAT v3 as a proposed recommendation. Since the IRI will not
  be changing, the DCAT version is not mentioned in the title.
</commit_message>
<xml_diff>
--- a/code/vocab_csv/tech.xlsx
+++ b/code/vocab_csv/tech.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1311" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="536">
   <si>
     <t>Term</t>
   </si>
@@ -279,6 +279,18 @@
     <t>tech:IntendedUse</t>
   </si>
   <si>
+    <t>hasDocumentation</t>
+  </si>
+  <si>
+    <t>has documentation</t>
+  </si>
+  <si>
+    <t>Indicates documentation associated with technology</t>
+  </si>
+  <si>
+    <t>tech:Documentation</t>
+  </si>
+  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -1186,9 +1198,6 @@
   </si>
   <si>
     <t>Documentation that provides instructions for using, maintaining, developing, or performing other activities regarding the technology</t>
-  </si>
-  <si>
-    <t>tech:Documentation</t>
   </si>
   <si>
     <t>Guide</t>
@@ -2852,10 +2861,10 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -2870,13 +2879,13 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="22" t="s">
@@ -2916,16 +2925,16 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="E5" s="22" t="s">
         <v>60</v>
@@ -2964,16 +2973,16 @@
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="E6" s="22" t="s">
         <v>60</v>
@@ -3012,16 +3021,16 @@
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
+        <v>456</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>456</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>457</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>453</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>453</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>454</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>450</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>60</v>
@@ -3060,16 +3069,16 @@
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>60</v>
@@ -3108,16 +3117,16 @@
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="E9" s="22" t="s">
         <v>60</v>
@@ -3156,13 +3165,13 @@
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="22" t="s">
@@ -3300,10 +3309,10 @@
     </row>
     <row r="2">
       <c r="A2" s="38" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="39"/>
@@ -3322,13 +3331,13 @@
     </row>
     <row r="4">
       <c r="A4" s="38" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
       <c r="D4" s="40"/>
       <c r="E4" s="6" t="s">
@@ -3376,16 +3385,16 @@
     </row>
     <row r="6">
       <c r="A6" s="38" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>16</v>
@@ -3422,16 +3431,16 @@
     </row>
     <row r="7">
       <c r="A7" s="24" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>16</v>
@@ -3472,16 +3481,16 @@
     </row>
     <row r="8">
       <c r="A8" s="17" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="C8" s="17" t="s">
+        <v>477</v>
+      </c>
+      <c r="D8" s="25" t="s">
         <v>474</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>471</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>16</v>
@@ -3518,16 +3527,16 @@
     </row>
     <row r="9">
       <c r="A9" s="17" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>16</v>
@@ -3564,16 +3573,16 @@
     </row>
     <row r="10">
       <c r="A10" s="24" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>16</v>
@@ -3614,16 +3623,16 @@
     </row>
     <row r="12">
       <c r="A12" s="38" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>16</v>
@@ -3660,16 +3669,16 @@
     </row>
     <row r="13">
       <c r="A13" s="24" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>16</v>
@@ -3710,16 +3719,16 @@
     </row>
     <row r="14">
       <c r="A14" s="6" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="C14" s="6" t="s">
+        <v>491</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>488</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>485</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>16</v>
@@ -3756,16 +3765,16 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>16</v>
@@ -3802,16 +3811,16 @@
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>16</v>
@@ -3848,16 +3857,16 @@
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>16</v>
@@ -3894,16 +3903,16 @@
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>502</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>498</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>498</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>499</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>495</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>16</v>
@@ -3940,16 +3949,16 @@
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>16</v>
@@ -3986,13 +3995,13 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="6" t="s">
@@ -4033,16 +4042,16 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>507</v>
+        <v>510</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>16</v>
@@ -4079,16 +4088,16 @@
     </row>
     <row r="25">
       <c r="A25" s="6" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>16</v>
@@ -4125,16 +4134,16 @@
     </row>
     <row r="26">
       <c r="A26" s="6" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>16</v>
@@ -4171,16 +4180,16 @@
     </row>
     <row r="27">
       <c r="A27" s="6" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="C27" s="6" t="s">
+        <v>521</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>518</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>515</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>16</v>
@@ -4217,16 +4226,16 @@
     </row>
     <row r="28">
       <c r="A28" s="6" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>16</v>
@@ -4263,16 +4272,16 @@
     </row>
     <row r="29">
       <c r="A29" s="6" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>16</v>
@@ -4309,16 +4318,16 @@
     </row>
     <row r="30">
       <c r="A30" s="6" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>16</v>
@@ -4456,27 +4465,27 @@
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="B2" s="5"/>
       <c r="J2" s="10" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
     </row>
     <row r="6">
@@ -5305,15 +5314,59 @@
       <c r="AB8" s="7"/>
     </row>
     <row r="9">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
+      <c r="A9" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="8">
+        <v>45472.0</v>
+      </c>
+      <c r="L9" s="7"/>
+      <c r="M9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="7"/>
+      <c r="AA9" s="7"/>
+      <c r="AB9" s="7"/>
     </row>
     <row r="11">
       <c r="C11" s="6"/>
     </row>
     <row r="14">
       <c r="A14" s="6" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B14" s="6"/>
     </row>
@@ -5486,26 +5539,26 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>16</v>
@@ -5515,7 +5568,7 @@
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N3" s="6" t="s">
         <v>39</v>
@@ -5526,16 +5579,16 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>94</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>90</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>16</v>
@@ -5545,7 +5598,7 @@
       </c>
       <c r="L4" s="8"/>
       <c r="M4" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N4" s="6" t="s">
         <v>39</v>
@@ -5556,16 +5609,16 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>16</v>
@@ -5575,7 +5628,7 @@
       </c>
       <c r="L5" s="8"/>
       <c r="M5" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N5" s="6" t="s">
         <v>39</v>
@@ -5586,16 +5639,16 @@
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>16</v>
@@ -5605,7 +5658,7 @@
       </c>
       <c r="L6" s="8"/>
       <c r="M6" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N6" s="6" t="s">
         <v>39</v>
@@ -5616,16 +5669,16 @@
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>16</v>
@@ -5635,7 +5688,7 @@
       </c>
       <c r="L7" s="8"/>
       <c r="M7" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N7" s="6" t="s">
         <v>39</v>
@@ -5646,16 +5699,16 @@
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>16</v>
@@ -5665,7 +5718,7 @@
       </c>
       <c r="L8" s="8"/>
       <c r="M8" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N8" s="6" t="s">
         <v>39</v>
@@ -5676,16 +5729,16 @@
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>16</v>
@@ -5695,7 +5748,7 @@
       </c>
       <c r="L9" s="8"/>
       <c r="M9" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N9" s="6" t="s">
         <v>39</v>
@@ -5706,16 +5759,16 @@
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>16</v>
@@ -5725,7 +5778,7 @@
       </c>
       <c r="L10" s="8"/>
       <c r="M10" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N10" s="6" t="s">
         <v>39</v>
@@ -5736,16 +5789,16 @@
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>16</v>
@@ -5755,7 +5808,7 @@
       </c>
       <c r="L11" s="8"/>
       <c r="M11" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N11" s="6" t="s">
         <v>39</v>
@@ -5766,16 +5819,16 @@
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>16</v>
@@ -5785,7 +5838,7 @@
       </c>
       <c r="L12" s="8"/>
       <c r="M12" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N12" s="6" t="s">
         <v>39</v>
@@ -5796,16 +5849,16 @@
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>16</v>
@@ -5814,7 +5867,7 @@
         <v>44727.0</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N13" s="6" t="s">
         <v>39</v>
@@ -5825,16 +5878,16 @@
     </row>
     <row r="14">
       <c r="A14" s="18" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>16</v>
@@ -5844,12 +5897,12 @@
       <c r="H14" s="21"/>
       <c r="I14" s="21"/>
       <c r="J14" s="18" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="K14" s="21"/>
       <c r="L14" s="21"/>
       <c r="M14" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N14" s="21"/>
       <c r="O14" s="21"/>
@@ -5872,18 +5925,18 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>16</v>
@@ -5892,7 +5945,7 @@
         <v>44727.0</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N17" s="6" t="s">
         <v>39</v>
@@ -5903,13 +5956,13 @@
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>16</v>
@@ -5919,7 +5972,7 @@
       </c>
       <c r="L18" s="8"/>
       <c r="M18" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N18" s="6" t="s">
         <v>39</v>
@@ -5930,13 +5983,13 @@
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>16</v>
@@ -5946,7 +5999,7 @@
       </c>
       <c r="L19" s="8"/>
       <c r="M19" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N19" s="6" t="s">
         <v>39</v>
@@ -5957,13 +6010,13 @@
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>16</v>
@@ -5973,7 +6026,7 @@
       </c>
       <c r="L20" s="8"/>
       <c r="M20" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N20" s="6" t="s">
         <v>39</v>
@@ -5984,13 +6037,13 @@
     </row>
     <row r="21">
       <c r="A21" s="6" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>16</v>
@@ -6000,7 +6053,7 @@
       </c>
       <c r="L21" s="8"/>
       <c r="M21" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N21" s="6" t="s">
         <v>39</v>
@@ -6011,13 +6064,13 @@
     </row>
     <row r="22">
       <c r="A22" s="6" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>16</v>
@@ -6027,7 +6080,7 @@
       </c>
       <c r="L22" s="8"/>
       <c r="M22" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N22" s="6" t="s">
         <v>39</v>
@@ -6038,10 +6091,10 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="22"/>
@@ -6050,16 +6103,16 @@
     </row>
     <row r="25">
       <c r="A25" s="6" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>16</v>
@@ -6068,7 +6121,7 @@
         <v>44727.0</v>
       </c>
       <c r="M25" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N25" s="6" t="s">
         <v>39</v>
@@ -6079,16 +6132,16 @@
     </row>
     <row r="26">
       <c r="A26" s="6" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>16</v>
@@ -6097,7 +6150,7 @@
         <v>44727.0</v>
       </c>
       <c r="M26" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N26" s="6" t="s">
         <v>39</v>
@@ -6108,16 +6161,16 @@
     </row>
     <row r="27">
       <c r="A27" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="D27" s="22" t="s">
         <v>155</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="D27" s="22" t="s">
-        <v>151</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>16</v>
@@ -6126,7 +6179,7 @@
         <v>44727.0</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N27" s="6" t="s">
         <v>39</v>
@@ -6137,16 +6190,16 @@
     </row>
     <row r="28">
       <c r="A28" s="6" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>16</v>
@@ -6155,7 +6208,7 @@
         <v>44727.0</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N28" s="6" t="s">
         <v>39</v>
@@ -6166,10 +6219,10 @@
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -6200,16 +6253,16 @@
     </row>
     <row r="31">
       <c r="A31" s="6" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>16</v>
@@ -6218,10 +6271,10 @@
         <v>44727.0</v>
       </c>
       <c r="M31" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N31" s="6" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="O31" s="9" t="s">
         <v>28</v>
@@ -6229,16 +6282,16 @@
     </row>
     <row r="32">
       <c r="A32" s="6" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C32" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="D32" s="6" t="s">
         <v>168</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>164</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>16</v>
@@ -6247,10 +6300,10 @@
         <v>44727.0</v>
       </c>
       <c r="M32" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N32" s="6" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="O32" s="9" t="s">
         <v>28</v>
@@ -6258,16 +6311,16 @@
     </row>
     <row r="33">
       <c r="A33" s="6" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>16</v>
@@ -6276,10 +6329,10 @@
         <v>44727.0</v>
       </c>
       <c r="M33" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="O33" s="9" t="s">
         <v>28</v>
@@ -6287,16 +6340,16 @@
     </row>
     <row r="34">
       <c r="A34" s="6" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>16</v>
@@ -6305,10 +6358,10 @@
         <v>44727.0</v>
       </c>
       <c r="M34" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N34" s="6" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="O34" s="9" t="s">
         <v>28</v>
@@ -6316,16 +6369,16 @@
     </row>
     <row r="35">
       <c r="A35" s="6" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>16</v>
@@ -6334,10 +6387,10 @@
         <v>44727.0</v>
       </c>
       <c r="M35" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N35" s="6" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="O35" s="9" t="s">
         <v>28</v>
@@ -6345,16 +6398,16 @@
     </row>
     <row r="36">
       <c r="A36" s="6" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>16</v>
@@ -6363,10 +6416,10 @@
         <v>44727.0</v>
       </c>
       <c r="M36" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N36" s="6" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="O36" s="9" t="s">
         <v>28</v>
@@ -6374,37 +6427,37 @@
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="K38" s="8"/>
     </row>
     <row r="39">
       <c r="A39" s="6" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>16</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="K39" s="8">
         <v>44727.0</v>
       </c>
       <c r="M39" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N39" s="6" t="s">
         <v>39</v>
@@ -6415,28 +6468,28 @@
     </row>
     <row r="40">
       <c r="A40" s="6" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="C40" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="D40" s="6" t="s">
         <v>190</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>186</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>16</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="K40" s="8">
         <v>44727.0</v>
       </c>
       <c r="M40" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N40" s="6" t="s">
         <v>39</v>
@@ -6447,21 +6500,21 @@
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="24" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="D43" s="25" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>16</v>
@@ -6470,7 +6523,7 @@
         <v>44727.0</v>
       </c>
       <c r="M43" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N43" s="6" t="s">
         <v>39</v>
@@ -6481,16 +6534,16 @@
     </row>
     <row r="44">
       <c r="A44" s="26" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="D44" s="28" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="E44" s="21" t="s">
         <v>16</v>
@@ -6505,7 +6558,7 @@
       </c>
       <c r="L44" s="21"/>
       <c r="M44" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N44" s="21" t="s">
         <v>39</v>
@@ -6531,16 +6584,16 @@
     </row>
     <row r="45">
       <c r="A45" s="26" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="C45" s="27" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="D45" s="31" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="E45" s="21" t="s">
         <v>16</v>
@@ -6555,7 +6608,7 @@
       </c>
       <c r="L45" s="21"/>
       <c r="M45" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N45" s="21" t="s">
         <v>39</v>
@@ -6581,16 +6634,16 @@
     </row>
     <row r="46">
       <c r="A46" s="26" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="C46" s="27" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="D46" s="31" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="E46" s="21" t="s">
         <v>16</v>
@@ -6605,7 +6658,7 @@
       </c>
       <c r="L46" s="21"/>
       <c r="M46" s="6" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="N46" s="21" t="s">
         <v>39</v>
@@ -6879,10 +6932,10 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -6891,19 +6944,19 @@
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="K3" s="8"/>
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="6" t="s">
@@ -6945,13 +6998,13 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="6" t="s">
@@ -6993,13 +7046,13 @@
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="6" t="s">
@@ -7041,13 +7094,13 @@
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="6" t="s">
@@ -7089,13 +7142,13 @@
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="6" t="s">
@@ -7105,7 +7158,7 @@
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="6" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="J8" s="7"/>
       <c r="K8" s="8">
@@ -7139,13 +7192,13 @@
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="6" t="s">
@@ -7187,13 +7240,13 @@
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="6" t="s">
@@ -7235,13 +7288,13 @@
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="6" t="s">
@@ -7287,16 +7340,16 @@
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>68</v>
@@ -7335,16 +7388,16 @@
     </row>
     <row r="14">
       <c r="A14" s="6" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>68</v>
@@ -7383,16 +7436,16 @@
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>68</v>
@@ -7431,16 +7484,16 @@
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>240</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>236</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>68</v>
@@ -7479,16 +7532,16 @@
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>68</v>
@@ -7527,16 +7580,16 @@
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>68</v>
@@ -7575,16 +7628,16 @@
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>68</v>
@@ -7623,16 +7676,16 @@
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>68</v>
@@ -7650,7 +7703,7 @@
         <v>26</v>
       </c>
       <c r="N20" s="6" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="O20" s="7"/>
       <c r="P20" s="7"/>
@@ -7671,16 +7724,16 @@
     </row>
     <row r="21">
       <c r="A21" s="6" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>68</v>
@@ -7698,7 +7751,7 @@
         <v>26</v>
       </c>
       <c r="N21" s="6" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="O21" s="7"/>
       <c r="P21" s="7"/>
@@ -7719,16 +7772,16 @@
     </row>
     <row r="22">
       <c r="A22" s="6" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>68</v>
@@ -7746,7 +7799,7 @@
         <v>26</v>
       </c>
       <c r="N22" s="6" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="O22" s="7"/>
       <c r="P22" s="7"/>
@@ -7885,10 +7938,10 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -7903,24 +7956,24 @@
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="6" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
       <c r="J4" s="6" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="K4" s="8">
         <v>45421.0</v>
@@ -7954,24 +8007,24 @@
     </row>
     <row r="5">
       <c r="A5" s="17" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="6" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="6" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="K5" s="8">
         <v>45421.0</v>
@@ -8001,26 +8054,26 @@
     </row>
     <row r="6">
       <c r="A6" s="17" t="s">
+        <v>274</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>274</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>270</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>270</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>266</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="6" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="K6" s="8">
         <v>45421.0</v>
@@ -8054,24 +8107,24 @@
     </row>
     <row r="7">
       <c r="A7" s="17" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="6" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
       <c r="J7" s="6" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="K7" s="8">
         <v>45421.0</v>
@@ -8101,26 +8154,26 @@
     </row>
     <row r="8">
       <c r="A8" s="17" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="6" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="K8" s="8">
         <v>45421.0</v>
@@ -8154,24 +8207,24 @@
     </row>
     <row r="9">
       <c r="A9" s="17" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="6" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
       <c r="J9" s="6" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="K9" s="8">
         <v>45421.0</v>
@@ -8205,24 +8258,24 @@
     </row>
     <row r="10">
       <c r="A10" s="32" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="6" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
       <c r="J10" s="32" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="K10" s="8">
         <v>45421.0</v>
@@ -8252,24 +8305,24 @@
     </row>
     <row r="11">
       <c r="A11" s="32" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="6" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
       <c r="H11" s="21"/>
       <c r="I11" s="21"/>
       <c r="J11" s="21" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="K11" s="8">
         <v>45421.0</v>
@@ -8299,24 +8352,24 @@
     </row>
     <row r="12">
       <c r="A12" s="32" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="6" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="21"/>
       <c r="I12" s="21"/>
       <c r="J12" s="21" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="K12" s="8">
         <v>45421.0</v>
@@ -8346,24 +8399,24 @@
     </row>
     <row r="13">
       <c r="A13" s="32" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="6" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="21"/>
       <c r="H13" s="21"/>
       <c r="I13" s="21"/>
       <c r="J13" s="21" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="K13" s="8">
         <v>45421.0</v>
@@ -8393,24 +8446,24 @@
     </row>
     <row r="14">
       <c r="A14" s="32" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="6" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
       <c r="I14" s="21"/>
       <c r="J14" s="21" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="K14" s="8">
         <v>45421.0</v>
@@ -8440,24 +8493,24 @@
     </row>
     <row r="15">
       <c r="A15" s="32" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="6" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="21"/>
       <c r="H15" s="21"/>
       <c r="I15" s="21"/>
       <c r="J15" s="21" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="K15" s="8">
         <v>45421.0</v>
@@ -8487,24 +8540,24 @@
     </row>
     <row r="16">
       <c r="A16" s="32" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="6" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="21"/>
       <c r="H16" s="21"/>
       <c r="I16" s="21"/>
       <c r="J16" s="21" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="K16" s="8">
         <v>45421.0</v>
@@ -8534,24 +8587,24 @@
     </row>
     <row r="17">
       <c r="A17" s="32" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="6" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="21"/>
       <c r="H17" s="21"/>
       <c r="I17" s="21"/>
       <c r="J17" s="21" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="K17" s="8">
         <v>45421.0</v>
@@ -8581,26 +8634,26 @@
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="6" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="6" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="K18" s="8">
         <v>45421.0</v>
@@ -8630,26 +8683,26 @@
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
       <c r="J19" s="6" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="K19" s="8">
         <v>45421.0</v>
@@ -8679,26 +8732,26 @@
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
       <c r="J20" s="6" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="K20" s="8">
         <v>45421.0</v>
@@ -8728,26 +8781,26 @@
     </row>
     <row r="21">
       <c r="A21" s="6" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>308</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>303</v>
-      </c>
       <c r="E21" s="6" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
       <c r="J21" s="6" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="K21" s="8">
         <v>45421.0</v>
@@ -8777,17 +8830,17 @@
     </row>
     <row r="22">
       <c r="A22" s="6" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="6" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
@@ -8822,17 +8875,17 @@
     </row>
     <row r="23">
       <c r="A23" s="6" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="6" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
@@ -8867,23 +8920,23 @@
     </row>
     <row r="24">
       <c r="A24" s="6" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="6" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
       <c r="I24" s="6" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="J24" s="7"/>
       <c r="K24" s="8">
@@ -9028,22 +9081,22 @@
     </row>
     <row r="2">
       <c r="A2" s="17" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="G2" s="34"/>
       <c r="H2" s="34"/>
@@ -9076,22 +9129,22 @@
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="G3" s="34"/>
       <c r="H3" s="34"/>
@@ -9124,22 +9177,22 @@
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="33" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="G4" s="34"/>
       <c r="H4" s="34"/>
@@ -9172,22 +9225,22 @@
     </row>
     <row r="5">
       <c r="A5" s="17" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="33" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="G5" s="34"/>
       <c r="H5" s="34"/>
@@ -9220,22 +9273,22 @@
     </row>
     <row r="6">
       <c r="A6" s="17" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
@@ -9268,22 +9321,22 @@
     </row>
     <row r="7">
       <c r="A7" s="17" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -9316,22 +9369,22 @@
     </row>
     <row r="8">
       <c r="A8" s="32" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
@@ -9364,22 +9417,22 @@
     </row>
     <row r="9">
       <c r="A9" s="32" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
@@ -9412,22 +9465,22 @@
     </row>
     <row r="10">
       <c r="A10" s="32" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
@@ -9460,22 +9513,22 @@
     </row>
     <row r="11">
       <c r="A11" s="32" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
@@ -9508,22 +9561,22 @@
     </row>
     <row r="12">
       <c r="A12" s="32" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
@@ -9556,22 +9609,22 @@
     </row>
     <row r="13">
       <c r="A13" s="32" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
@@ -9604,22 +9657,22 @@
     </row>
     <row r="14">
       <c r="A14" s="32" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
@@ -9652,22 +9705,22 @@
     </row>
     <row r="15">
       <c r="A15" s="32" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
@@ -9700,22 +9753,22 @@
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
@@ -9748,22 +9801,22 @@
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
@@ -9796,22 +9849,22 @@
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
@@ -9844,22 +9897,22 @@
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
@@ -10007,10 +10060,10 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -10025,17 +10078,17 @@
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="6" t="s">
-        <v>388</v>
+        <v>88</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -10072,17 +10125,17 @@
     </row>
     <row r="5">
       <c r="A5" s="17" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="6" t="s">
-        <v>388</v>
+        <v>88</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -10117,17 +10170,17 @@
     </row>
     <row r="6">
       <c r="A6" s="17" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="6" t="s">
-        <v>388</v>
+        <v>88</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -10164,17 +10217,17 @@
     </row>
     <row r="7">
       <c r="A7" s="17" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="6" t="s">
-        <v>388</v>
+        <v>88</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -10209,17 +10262,17 @@
     </row>
     <row r="8">
       <c r="A8" s="17" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="6" t="s">
-        <v>388</v>
+        <v>88</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
@@ -10254,19 +10307,19 @@
     </row>
     <row r="9">
       <c r="A9" s="17" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>388</v>
+        <v>88</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
@@ -10301,19 +10354,19 @@
     </row>
     <row r="10">
       <c r="A10" s="32" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="C10" s="32" t="s">
+        <v>406</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>403</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>400</v>
-      </c>
       <c r="E10" s="6" t="s">
-        <v>388</v>
+        <v>88</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
@@ -10658,10 +10711,10 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -10670,13 +10723,13 @@
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="K3" s="8"/>
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B4" s="17"/>
       <c r="C4" s="17"/>
@@ -10687,7 +10740,7 @@
     </row>
     <row r="5">
       <c r="A5" s="17" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
@@ -10696,16 +10749,16 @@
     </row>
     <row r="6">
       <c r="A6" s="17" t="s">
+        <v>410</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>411</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>412</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>407</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>408</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>409</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>404</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>25</v>
@@ -10743,16 +10796,16 @@
     </row>
     <row r="7">
       <c r="A7" s="17" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>25</v>
@@ -10792,17 +10845,17 @@
     </row>
     <row r="8">
       <c r="A8" s="17" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="6" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
@@ -10837,17 +10890,17 @@
     </row>
     <row r="9">
       <c r="A9" s="17" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="6" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
@@ -10882,16 +10935,16 @@
     </row>
     <row r="10">
       <c r="A10" s="32" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>25</v>
@@ -10929,17 +10982,17 @@
     </row>
     <row r="11">
       <c r="A11" s="32" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="6" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
@@ -10974,17 +11027,17 @@
     </row>
     <row r="12">
       <c r="A12" s="32" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="6" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
@@ -11019,16 +11072,16 @@
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>25</v>
@@ -11183,22 +11236,22 @@
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -11233,22 +11286,22 @@
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -11279,22 +11332,22 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
@@ -11328,7 +11381,7 @@
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B9" s="6"/>
     </row>

</xml_diff>

<commit_message>
Changes tech:ProvisionMethod ; closes #207
- Changes `tech:ProvisionMethod` concept by adding a prefix to
  distinguish it from the technology concept
- e.g. `tech:System` is not a kind of technology, and
  `tech:ProvidedAsSystem` is a provision method
</commit_message>
<xml_diff>
--- a/code/vocab_csv/tech.xlsx
+++ b/code/vocab_csv/tech.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1843" uniqueCount="790">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1843" uniqueCount="792">
   <si>
     <t>Term</t>
   </si>
@@ -594,10 +594,10 @@
     <t>TechnologyProvisionMethod</t>
   </si>
   <si>
-    <t>FixedUseProvision</t>
-  </si>
-  <si>
-    <t>Fixed Use Provision</t>
+    <t>ProvidedAsFixedUse</t>
+  </si>
+  <si>
+    <t>Provided as Fixed UseProvision</t>
   </si>
   <si>
     <t>Technology provided for using a fixed number of times</t>
@@ -606,1222 +606,1228 @@
     <t>modified</t>
   </si>
   <si>
-    <t>SubscriptionProvision</t>
-  </si>
-  <si>
-    <t>Subscription Provision</t>
+    <t>ProvidedAsSubscription</t>
+  </si>
+  <si>
+    <t>Provided as SubscriptionProvision</t>
   </si>
   <si>
     <t xml:space="preserve">Technology that is provided or used as a periodic subscription </t>
   </si>
   <si>
-    <t>ProductProvision</t>
-  </si>
-  <si>
-    <t>Product Provision</t>
+    <t>ProvidedAsProduct</t>
+  </si>
+  <si>
+    <t>Provided as ProductProvision</t>
   </si>
   <si>
     <t>Technology provided as a product</t>
   </si>
   <si>
-    <t>GoodsProvision</t>
-  </si>
-  <si>
-    <t>Goods Provision</t>
+    <t>ProvidedAsGoods</t>
+  </si>
+  <si>
+    <t>Provided as GoodsProvision</t>
   </si>
   <si>
     <t>Technology provided or used as goods</t>
   </si>
   <si>
-    <t>ServiceProvision</t>
-  </si>
-  <si>
-    <t>Service Provision</t>
+    <t>ProvidedAsService</t>
+  </si>
+  <si>
+    <t>Provided as ServiceProvision</t>
   </si>
   <si>
     <t>Technology provided or used as service(s)</t>
   </si>
   <si>
-    <t>AlgorithmicProvision</t>
-  </si>
-  <si>
-    <t>Algorithmic Provision</t>
+    <t>ProvidedAsAlgorithmic</t>
+  </si>
+  <si>
+    <t>Provided as AlgorithmicProvision</t>
   </si>
   <si>
     <t>Technology provided as an algorithm or method</t>
   </si>
   <si>
-    <t>SystemProvision</t>
-  </si>
-  <si>
-    <t>System Provision</t>
+    <t>ProvidedAsSystem</t>
+  </si>
+  <si>
+    <t>Provided as SystemProvision</t>
   </si>
   <si>
     <t>Technology provided as a system</t>
   </si>
   <si>
-    <t>ComponentProvision</t>
-  </si>
-  <si>
-    <t>Component Provision</t>
+    <t>ProvidedAsComponent</t>
+  </si>
+  <si>
+    <t>Provided as ComponentProvision</t>
   </si>
   <si>
     <t>Technology provided as a component</t>
   </si>
   <si>
-    <t>CloudServiceProvision</t>
+    <t>ProvidedAsCloudService</t>
+  </si>
+  <si>
+    <t>Provided as Cloud ServiceProvision</t>
+  </si>
+  <si>
+    <t>Technology provided as a cloud service</t>
+  </si>
+  <si>
+    <t>tech:ProvidedAsService</t>
+  </si>
+  <si>
+    <t>ProvidedAsIaaS</t>
+  </si>
+  <si>
+    <t>Provided as Infrastructure as a Service (IaaS)Provision</t>
+  </si>
+  <si>
+    <t>Technology provided as a cloud service consisting of managed infrastructure resources</t>
+  </si>
+  <si>
+    <t>tech:ProvidedAsCloudService</t>
+  </si>
+  <si>
+    <t>ProvidedAsPaaS</t>
+  </si>
+  <si>
+    <t>Provided as Platform as a Service (PaaS)Provision</t>
+  </si>
+  <si>
+    <t>Technology provided as a cloud service consisting of managed platform resources</t>
+  </si>
+  <si>
+    <t>ProvidedAsSaaS</t>
+  </si>
+  <si>
+    <t>Provided as Software as a Service (SaaS)Provision</t>
+  </si>
+  <si>
+    <t>Technology provided as a cloud service consisting of managed software resources</t>
+  </si>
+  <si>
+    <t>ProvidedAsCaaS</t>
+  </si>
+  <si>
+    <t>Provided as Compute as a Service (CaaS)Provision</t>
+  </si>
+  <si>
+    <t>Technology provided as a cloud service consisting of managed compute resources</t>
+  </si>
+  <si>
+    <t>ProvidedAsMBaaS</t>
+  </si>
+  <si>
+    <t>Provided as Mobile backend as a ServiceProvision</t>
+  </si>
+  <si>
+    <t>Technology provided as a cloud service consisting of managed 'backend' services for mobile users</t>
+  </si>
+  <si>
+    <t>ProvidedAsServerlessComputing</t>
+  </si>
+  <si>
+    <t>Provided as Serverless ComputingProvision</t>
+  </si>
+  <si>
+    <t>Technology provided as a cloud service consisting of fully managed servers for executing functions</t>
+  </si>
+  <si>
+    <t>ProvidedAsPrivateCloudService</t>
+  </si>
+  <si>
+    <t>Provided as Private Cloud ServiceProvision</t>
+  </si>
+  <si>
+    <t>Technology provided as a cloud service that is private</t>
+  </si>
+  <si>
+    <t>Tek Raj Chhetri</t>
+  </si>
+  <si>
+    <t>ProvidedAsPublicCloudService</t>
+  </si>
+  <si>
+    <t>Provided as Public Cloud ServiceProvision</t>
+  </si>
+  <si>
+    <t>Technology provided as a cloud service that is public</t>
+  </si>
+  <si>
+    <t>ProvidedAsHybridCloudService</t>
+  </si>
+  <si>
+    <t>Provided as Hybrid Cloud ServiceProvision</t>
+  </si>
+  <si>
+    <t>Technology provided as a cloud service that is both private and public in parts</t>
+  </si>
+  <si>
+    <t>tech:ProvidedAsPrivateCloudService,tech:ProvidedAsPublicCloudService</t>
+  </si>
+  <si>
+    <t>Proposed for v2.2</t>
+  </si>
+  <si>
+    <t>ConceptStage</t>
+  </si>
+  <si>
+    <t>Concept Stage</t>
+  </si>
+  <si>
+    <t>DevelopmentStage</t>
+  </si>
+  <si>
+    <t>Development Stage</t>
+  </si>
+  <si>
+    <t>ProductionStage</t>
+  </si>
+  <si>
+    <t>Production Stage</t>
+  </si>
+  <si>
+    <t>UtilisationStage</t>
+  </si>
+  <si>
+    <t>Utilisation Stage</t>
+  </si>
+  <si>
+    <t>SupportStage</t>
+  </si>
+  <si>
+    <t>Support Stage</t>
+  </si>
+  <si>
+    <t>RetirementStage</t>
+  </si>
+  <si>
+    <t>Retirement Stage</t>
+  </si>
+  <si>
+    <t>ChangeDescription</t>
+  </si>
+  <si>
+    <t>ChangeStatus</t>
+  </si>
+  <si>
+    <t>ChangeProposed</t>
+  </si>
+  <si>
+    <t>ChangeApproved</t>
+  </si>
+  <si>
+    <t>ChangeRequested</t>
+  </si>
+  <si>
+    <t>ChangeAuthorised</t>
+  </si>
+  <si>
+    <t>ChangeVerified</t>
+  </si>
+  <si>
+    <t>ChangePlanned</t>
+  </si>
+  <si>
+    <t>ChangePending</t>
+  </si>
+  <si>
+    <t>ChangeScheduled</t>
+  </si>
+  <si>
+    <t>ChangeOngoing</t>
+  </si>
+  <si>
+    <t>ChangeCompleted</t>
+  </si>
+  <si>
+    <t>ChangeFailed</t>
+  </si>
+  <si>
+    <t>ChangePaused</t>
+  </si>
+  <si>
+    <t>ChangeReverted</t>
+  </si>
+  <si>
+    <t>ChangeCategory</t>
+  </si>
+  <si>
+    <t>SystematicChangeCategory</t>
+  </si>
+  <si>
+    <t>SystematicChange</t>
+  </si>
+  <si>
+    <t>AdhocChange</t>
+  </si>
+  <si>
+    <t>PlannedChangeCategory</t>
+  </si>
+  <si>
+    <t>PlannedChange</t>
+  </si>
+  <si>
+    <t>Vague broad notion of change planned</t>
+  </si>
+  <si>
+    <t>UnplannedChange</t>
+  </si>
+  <si>
+    <t>Change that is not planned</t>
+  </si>
+  <si>
+    <t>PredeterminedChangeCategory</t>
+  </si>
+  <si>
+    <t>PredeterminedChange</t>
+  </si>
+  <si>
+    <t>Specific determination of change in terms of what to change or when to change - can include reaction to external factors</t>
+  </si>
+  <si>
+    <t>NonpredeterminedChange</t>
+  </si>
+  <si>
+    <t>Change that is not predetermined but is planned</t>
+  </si>
+  <si>
+    <t>IntendedChangeCategory</t>
+  </si>
+  <si>
+    <t>IntendedChange</t>
+  </si>
+  <si>
+    <t>UnintendedChange</t>
+  </si>
+  <si>
+    <t>RateOfChangeCategory</t>
+  </si>
+  <si>
+    <t>GradualChange</t>
+  </si>
+  <si>
+    <t>InstantaneousChange</t>
+  </si>
+  <si>
+    <t>ReversibilityOfChangeCategory</t>
+  </si>
+  <si>
+    <t>ReversibleChange</t>
+  </si>
+  <si>
+    <t>IrreversibleChange</t>
+  </si>
+  <si>
+    <t>TransformationChangeCategory</t>
+  </si>
+  <si>
+    <t>IncrementalChange</t>
+  </si>
+  <si>
+    <t>TransformativeChange</t>
+  </si>
+  <si>
+    <t>ControlOverChangeCategory</t>
+  </si>
+  <si>
+    <t>ControlledChange</t>
+  </si>
+  <si>
+    <t>UncontrolledChange</t>
+  </si>
+  <si>
+    <t>TemporalChangeCategory</t>
+  </si>
+  <si>
+    <t>TemporaryChange</t>
+  </si>
+  <si>
+    <t>LastingChange</t>
+  </si>
+  <si>
+    <t>Actors involved in technologies</t>
+  </si>
+  <si>
+    <t>Provider</t>
+  </si>
+  <si>
+    <t>Actor that provides Technology</t>
+  </si>
+  <si>
+    <t>tech:Actor</t>
+  </si>
+  <si>
+    <t>ISO/IEC 22989:2022</t>
+  </si>
+  <si>
+    <t>Producer</t>
+  </si>
+  <si>
+    <t>Actor that produces Technology</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>Actor that develops Technology</t>
+  </si>
+  <si>
+    <t>tech:Producer</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Actor that uses Technology directly or indirectly by providing it to Users</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Actor that uses Technology</t>
+  </si>
+  <si>
+    <t>tech:Customer</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Actor that is subjected to the use or impact of Technology</t>
+  </si>
+  <si>
+    <t>Subject can be a human or non-human entity. To explicitly indicate that the subject is a human, and to reuse DPV's human subject taxonomy, the tech:Subject should also be defined as an instance or category of dpv:HumanSubject</t>
+  </si>
+  <si>
+    <t>Deployer</t>
+  </si>
+  <si>
+    <t>Actor that deploys Technology</t>
+  </si>
+  <si>
+    <t>AI Act</t>
+  </si>
+  <si>
+    <t>Designer</t>
+  </si>
+  <si>
+    <t>Actor that designs Technology</t>
+  </si>
+  <si>
+    <t>DGA 26.3</t>
+  </si>
+  <si>
+    <t>Installer</t>
+  </si>
+  <si>
+    <t>Actor that installs Technology</t>
+  </si>
+  <si>
+    <t>Maintainer</t>
+  </si>
+  <si>
+    <t>Actor that maintains Technology</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>Actor that manufactures Technology</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Actor that owns Technology</t>
+  </si>
+  <si>
+    <t>Purchaser</t>
+  </si>
+  <si>
+    <t>Actor that purchases Technology</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>Actor that supplies Technology</t>
+  </si>
+  <si>
+    <t>Partner</t>
+  </si>
+  <si>
+    <t>Actor that provides services in the context of Technology</t>
+  </si>
+  <si>
+    <t>"Partner" is a vague term and should not be used - instead the more specific terms provided in this vocabulary should be used. Partner refers to entities that provide services for the technology (as opposed to for using the technology) - for example to further develop or refine it, or to test or audit it.</t>
+  </si>
+  <si>
+    <t>Evaluator</t>
+  </si>
+  <si>
+    <t>Actor that evaluates the performance of Technology</t>
+  </si>
+  <si>
+    <t>tech:Partner</t>
+  </si>
+  <si>
+    <t>Auditor</t>
+  </si>
+  <si>
+    <t>Actor that audits Technology for conformance to policies, standards, or legal requirements</t>
+  </si>
+  <si>
+    <t>SystemIntegrator</t>
+  </si>
+  <si>
+    <t>System Integrator</t>
+  </si>
+  <si>
+    <t>Actor that integrates Technology in to (larger) systems</t>
+  </si>
+  <si>
+    <t>Importer</t>
+  </si>
+  <si>
+    <t>Actor that imports the Technology within a jurisdiction</t>
+  </si>
+  <si>
+    <t>Distributor</t>
+  </si>
+  <si>
+    <t>Actor that distributes the Technology</t>
+  </si>
+  <si>
+    <t>Operator</t>
+  </si>
+  <si>
+    <t>Actor that operates the Technology</t>
+  </si>
+  <si>
+    <t>Operator and User are similar concepts but may refer to different actors, for example in the scenario where the user determines what actions to perform on the technology and the operator executes these actions by operating the technology</t>
+  </si>
+  <si>
+    <t>hasProvider</t>
+  </si>
+  <si>
+    <t>has provider</t>
+  </si>
+  <si>
+    <t>Indicates technology provider</t>
+  </si>
+  <si>
+    <t>tech:Provider</t>
+  </si>
+  <si>
+    <t>tech:hasActor</t>
+  </si>
+  <si>
+    <t>hasProducer</t>
+  </si>
+  <si>
+    <t>has producer</t>
+  </si>
+  <si>
+    <t>Indicates technology producer</t>
+  </si>
+  <si>
+    <t>hasDeveloper</t>
+  </si>
+  <si>
+    <t>has developer</t>
+  </si>
+  <si>
+    <t>Indicates technology developer</t>
+  </si>
+  <si>
+    <t>tech:Developer</t>
+  </si>
+  <si>
+    <t>hasCustomer</t>
+  </si>
+  <si>
+    <t>has customer</t>
+  </si>
+  <si>
+    <t>Indicates technology customer</t>
+  </si>
+  <si>
+    <t>hasUser</t>
+  </si>
+  <si>
+    <t>has user</t>
+  </si>
+  <si>
+    <t>Indicates technology user</t>
+  </si>
+  <si>
+    <t>tech:User</t>
+  </si>
+  <si>
+    <t>hasSubject</t>
+  </si>
+  <si>
+    <t>has subject</t>
+  </si>
+  <si>
+    <t>Indicates technology subject</t>
+  </si>
+  <si>
+    <t>tech:Subject</t>
+  </si>
+  <si>
+    <t>hasDeployer</t>
+  </si>
+  <si>
+    <t>has deployer</t>
+  </si>
+  <si>
+    <t>Indicates technology deployer</t>
+  </si>
+  <si>
+    <t>tech:Deployer</t>
+  </si>
+  <si>
+    <t>hasDesigner</t>
+  </si>
+  <si>
+    <t>has designer</t>
+  </si>
+  <si>
+    <t>Indicates technology designer</t>
+  </si>
+  <si>
+    <t>tech:Designer</t>
+  </si>
+  <si>
+    <t>hasInstaller</t>
+  </si>
+  <si>
+    <t>has installer</t>
+  </si>
+  <si>
+    <t>Indicates technology installer</t>
+  </si>
+  <si>
+    <t>tech:Installer</t>
+  </si>
+  <si>
+    <t>hasMaintainer</t>
+  </si>
+  <si>
+    <t>has maintainer</t>
+  </si>
+  <si>
+    <t>Indicates technology maintainer</t>
+  </si>
+  <si>
+    <t>tech:Maintainer</t>
+  </si>
+  <si>
+    <t>hasManufacturer</t>
+  </si>
+  <si>
+    <t>has manufacturer</t>
+  </si>
+  <si>
+    <t>Indicates technology manufacturer</t>
+  </si>
+  <si>
+    <t>tech:Manufacturer</t>
+  </si>
+  <si>
+    <t>hasOwner</t>
+  </si>
+  <si>
+    <t>has owner</t>
+  </si>
+  <si>
+    <t>Indicates technology owner</t>
+  </si>
+  <si>
+    <t>tech:Owner</t>
+  </si>
+  <si>
+    <t>hasPurchaser</t>
+  </si>
+  <si>
+    <t>has purchaser</t>
+  </si>
+  <si>
+    <t>Indicates technology purchaser</t>
+  </si>
+  <si>
+    <t>tech:Purchaser</t>
+  </si>
+  <si>
+    <t>hasSupplier</t>
+  </si>
+  <si>
+    <t>has supplier</t>
+  </si>
+  <si>
+    <t>Indicates technology supplier</t>
+  </si>
+  <si>
+    <t>tech:Supplier</t>
+  </si>
+  <si>
+    <t>hasPartner</t>
+  </si>
+  <si>
+    <t>has partner</t>
+  </si>
+  <si>
+    <t>Indicates technology partner</t>
+  </si>
+  <si>
+    <t>hasEvaluator</t>
+  </si>
+  <si>
+    <t>has evaluator</t>
+  </si>
+  <si>
+    <t>Indicates technology evaluator</t>
+  </si>
+  <si>
+    <t>tech:Evaluator</t>
+  </si>
+  <si>
+    <t>hasAuditor</t>
+  </si>
+  <si>
+    <t>has auditor</t>
+  </si>
+  <si>
+    <t>Indicates technology auditor</t>
+  </si>
+  <si>
+    <t>tech:Auditor</t>
+  </si>
+  <si>
+    <t>hasSystemIntegrator</t>
+  </si>
+  <si>
+    <t>has system integrator</t>
+  </si>
+  <si>
+    <t>Indicates technology system integrator</t>
+  </si>
+  <si>
+    <t>tech:SystemIntegrator</t>
+  </si>
+  <si>
+    <t>Manual</t>
+  </si>
+  <si>
+    <t>Documentation that provides instructions for using, maintaining, developing, or performing other activities regarding the technology</t>
+  </si>
+  <si>
+    <t>Guide</t>
+  </si>
+  <si>
+    <t>Documentation that provides guidance regarding the technology</t>
+  </si>
+  <si>
+    <t>Instructions</t>
+  </si>
+  <si>
+    <t>Instructions related to technology</t>
+  </si>
+  <si>
+    <t>Specification</t>
+  </si>
+  <si>
+    <t>Documentation that specifies requirements that must be satisfied by the technology</t>
+  </si>
+  <si>
+    <t>Plan</t>
+  </si>
+  <si>
+    <t>Plan associated with using, maintaining, developing, or performing other activities associated with technology</t>
+  </si>
+  <si>
+    <t>TestingPlan</t>
+  </si>
+  <si>
+    <t>Testing Plan</t>
+  </si>
+  <si>
+    <t>Plan associated with testing technology</t>
+  </si>
+  <si>
+    <t>tech:Plan</t>
+  </si>
+  <si>
+    <t>DevelopmentPlan</t>
+  </si>
+  <si>
+    <t>Development Plan</t>
+  </si>
+  <si>
+    <t>Plan associated with developing technology</t>
+  </si>
+  <si>
+    <t>dpv:Status</t>
+  </si>
+  <si>
+    <t>DevelopmentStatus</t>
+  </si>
+  <si>
+    <t>DeploymentStatus</t>
+  </si>
+  <si>
+    <t>TechnologyStatus</t>
+  </si>
+  <si>
+    <t>Technology Status</t>
+  </si>
+  <si>
+    <t>Status associated with development, deployment, and use of technology</t>
+  </si>
+  <si>
+    <t>MarketAvailabilityStatus</t>
+  </si>
+  <si>
+    <t>Market Availability Status</t>
+  </si>
+  <si>
+    <t>Status indicating whether Technology is available on the market</t>
+  </si>
+  <si>
+    <t>tech:TechnologyStatus</t>
+  </si>
+  <si>
+    <t>MarketAvailable</t>
+  </si>
+  <si>
+    <t>Market Available</t>
+  </si>
+  <si>
+    <t>Status indicating Technology is available on the market</t>
+  </si>
+  <si>
+    <t>tech:MarketAvailabilityStatus</t>
+  </si>
+  <si>
+    <t>MarketUnavailable</t>
+  </si>
+  <si>
+    <t>Market Unavailable</t>
+  </si>
+  <si>
+    <t>Status indicating Technology is unavailable on the market</t>
+  </si>
+  <si>
+    <t>ProvisionStatus</t>
+  </si>
+  <si>
+    <t>Provision Status</t>
+  </si>
+  <si>
+    <t>Status indicating whether Technology has been provided</t>
+  </si>
+  <si>
+    <t>Provided</t>
+  </si>
+  <si>
+    <t>Status indicating Technology has been provided</t>
+  </si>
+  <si>
+    <t>tech:ProvisionStatus</t>
+  </si>
+  <si>
+    <t>NotProvided</t>
+  </si>
+  <si>
+    <t>Not Provided</t>
+  </si>
+  <si>
+    <t>Status indicating Technology has not been provided</t>
+  </si>
+  <si>
+    <t>TechnologyReadinessLevel</t>
+  </si>
+  <si>
+    <t>Technology Readiness Level (TRL)</t>
+  </si>
+  <si>
+    <t>Indication of maturity of Technology (ISO 16290:2013)</t>
+  </si>
+  <si>
+    <t>hasTRL</t>
+  </si>
+  <si>
+    <t>has TRL</t>
+  </si>
+  <si>
+    <t>Indicates technology maturity level</t>
+  </si>
+  <si>
+    <t>tech:TechnologyReadinessLevel</t>
+  </si>
+  <si>
+    <t>dpv:hasStatus</t>
+  </si>
+  <si>
+    <t>hasMarketAvailabilityStatus</t>
+  </si>
+  <si>
+    <t>has market availability status</t>
+  </si>
+  <si>
+    <t>Indicates whether the technology is available on the market</t>
+  </si>
+  <si>
+    <t>hasProvisionStatus</t>
+  </si>
+  <si>
+    <t>has provision status</t>
+  </si>
+  <si>
+    <t>Indicates whether the technology has been provided</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>How technology communicates</t>
+  </si>
+  <si>
+    <t>Networking</t>
+  </si>
+  <si>
+    <t>Technology utilising networking</t>
+  </si>
+  <si>
+    <t>LocalNetwork</t>
+  </si>
+  <si>
+    <t>Local Network</t>
+  </si>
+  <si>
+    <t>Technology utilising local networking</t>
+  </si>
+  <si>
+    <t>tech:Networking</t>
+  </si>
+  <si>
+    <t>Internet</t>
+  </si>
+  <si>
+    <t>Technology utilising internet</t>
+  </si>
+  <si>
+    <t>WiFi</t>
+  </si>
+  <si>
+    <t>Technology utilising wifi wireless networking</t>
+  </si>
+  <si>
+    <t>Bluetooth</t>
+  </si>
+  <si>
+    <t>Technology utilising bluetooth</t>
+  </si>
+  <si>
+    <t>CellularNetwork</t>
+  </si>
+  <si>
+    <t>Cellular Network</t>
+  </si>
+  <si>
+    <t>Technology utilising cellular networking</t>
+  </si>
+  <si>
+    <t>GPS</t>
+  </si>
+  <si>
+    <t>Technology utilising GPS</t>
+  </si>
+  <si>
+    <t>Specific instances of technologies</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>Virtual parts or components of the technology such as programs and data</t>
+  </si>
+  <si>
+    <t>DataStorage</t>
+  </si>
+  <si>
+    <t>Data Storage</t>
+  </si>
+  <si>
+    <t>Technology associated with storage of data</t>
+  </si>
+  <si>
+    <t>tech:Software</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>A database, database management system (DBMS), or application database</t>
+  </si>
+  <si>
+    <t>tech:DataStorage</t>
+  </si>
+  <si>
+    <t>CloudStorage</t>
+  </si>
+  <si>
+    <t>Cloud Storage</t>
+  </si>
+  <si>
+    <t>Storage utilising cloud technologies</t>
+  </si>
+  <si>
+    <t>LocalStorage</t>
+  </si>
+  <si>
+    <t>Local Storage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Storage that is local (e.g. on device) </t>
+  </si>
+  <si>
+    <t>Cookie</t>
+  </si>
+  <si>
+    <t>A HTTP or web or internet cookie</t>
+  </si>
+  <si>
+    <t>tech:LocalStorage</t>
+  </si>
+  <si>
+    <t>Application</t>
+  </si>
+  <si>
+    <t>Application or Application Software</t>
+  </si>
+  <si>
+    <t>SmartphoneApplication</t>
+  </si>
+  <si>
+    <t>Smartphone Application</t>
+  </si>
+  <si>
+    <t>A computing or digital program on a smartphone device</t>
+  </si>
+  <si>
+    <t>tech:Application</t>
+  </si>
+  <si>
+    <t>AppStore</t>
+  </si>
+  <si>
+    <t>Application Store</t>
+  </si>
+  <si>
+    <t>An application or platform for distribution of other applications</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>Operating System (OS)</t>
+  </si>
+  <si>
+    <t>Software for managing hardware and other software</t>
+  </si>
+  <si>
+    <t>MSWindows</t>
+  </si>
+  <si>
+    <t>Microsoft Windows</t>
+  </si>
+  <si>
+    <t>Microsoft Windows operating system</t>
+  </si>
+  <si>
+    <t>tech:OS</t>
+  </si>
+  <si>
+    <t>iOS</t>
+  </si>
+  <si>
+    <t>iOS operating system</t>
+  </si>
+  <si>
+    <t>Android</t>
+  </si>
+  <si>
+    <t>Android operating system</t>
+  </si>
+  <si>
+    <t>GNULinux</t>
+  </si>
+  <si>
+    <t>GNU/Linux</t>
+  </si>
+  <si>
+    <t>GNU/Linux operating system</t>
+  </si>
+  <si>
+    <t>Hardware</t>
+  </si>
+  <si>
+    <t>Physical parts or components of the technology</t>
+  </si>
+  <si>
+    <t>Device</t>
+  </si>
+  <si>
+    <t>Device or computing device</t>
+  </si>
+  <si>
+    <t>tech:Hardware</t>
+  </si>
+  <si>
+    <t>PersonalComputer</t>
+  </si>
+  <si>
+    <t>Personal Computer (PC)</t>
+  </si>
+  <si>
+    <t>A computing device intended for individual use</t>
+  </si>
+  <si>
+    <t>tech:Device</t>
+  </si>
+  <si>
+    <t>LaptopPC</t>
+  </si>
+  <si>
+    <t>Laptop PC</t>
+  </si>
+  <si>
+    <t>A portal personal computer</t>
+  </si>
+  <si>
+    <t>tech:PersonalComputer</t>
+  </si>
+  <si>
+    <t>DesktopPC</t>
+  </si>
+  <si>
+    <t>Desktop PC</t>
+  </si>
+  <si>
+    <t>A non-portable or fixed personal computer</t>
+  </si>
+  <si>
+    <t>Telephone</t>
+  </si>
+  <si>
+    <t>MobilePhone</t>
+  </si>
+  <si>
+    <t>Mobile Phone</t>
+  </si>
+  <si>
+    <t>Mobile telephone</t>
+  </si>
+  <si>
+    <t>tech:Telephone</t>
+  </si>
+  <si>
+    <t>Smartphone</t>
+  </si>
+  <si>
+    <t>A combination of a mobile phone with computing capabilities similar to a PC</t>
+  </si>
+  <si>
+    <t>tech:MobilePhone,tech:PersonalComputer</t>
+  </si>
+  <si>
+    <t>IoT</t>
+  </si>
+  <si>
+    <t>Internet of Things (IoT)</t>
+  </si>
+  <si>
+    <t>IoT is the infrastructure of interconnected entities, people, systems and information resources together with services that process and react to information from the physical world and virtual world</t>
+  </si>
+  <si>
+    <t>IoTDevice</t>
+  </si>
+  <si>
+    <t>IoT Device</t>
+  </si>
+  <si>
+    <t>An entity of an IoT system that interacts and communicates with the physical world through sensing or actuating</t>
+  </si>
+  <si>
+    <t>tech:IoT,tech:Device</t>
+  </si>
+  <si>
+    <t>IoTSystem</t>
+  </si>
+  <si>
+    <t>IoT System</t>
+  </si>
+  <si>
+    <t>A specific system that is an implementation or application of the IoT framework and contains interconnected IoT devices and their communication network along with other hardware and software required for providing functionalities</t>
+  </si>
+  <si>
+    <t>tech:IoT,tech:System</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>A simplified representation or abstraction of a system, process, or concept</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>The carrying out of a specific task or set of tasks as a service</t>
+  </si>
+  <si>
+    <t>This concept is distinct from dpv:Service as it represents the notion of a technical service whereas dpv:Service can also refer to organisational, legal, social, and other meanings of service</t>
+  </si>
+  <si>
+    <t>Algorithm</t>
+  </si>
+  <si>
+    <t>A step-by-step set of instructions used to solve a problem or perform a computation</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+  <si>
+    <t>A collection of components that interact to achieve a specific goal or function</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>A self-contained part of a system that performs a specific function and interacts with other components</t>
+  </si>
+  <si>
+    <t>CloudService</t>
   </si>
   <si>
     <t>Cloud Service Provision</t>
   </si>
   <si>
-    <t>Technology provided as a cloud service</t>
-  </si>
-  <si>
-    <t>tech:ServiceProvision</t>
-  </si>
-  <si>
-    <t>IaaSProvision</t>
+    <t>A remotely accessible service delivered over the internet for providing resources, software, or infrastructure</t>
+  </si>
+  <si>
+    <t>Infrastructure</t>
   </si>
   <si>
     <t>Infrastructure as a Service (IaaS) Provision</t>
-  </si>
-  <si>
-    <t>Technology provided as a cloud service consisting of managed infrastructure resources</t>
-  </si>
-  <si>
-    <t>tech:CloudServiceProvision</t>
-  </si>
-  <si>
-    <t>PaaSProvision</t>
-  </si>
-  <si>
-    <t>Platform as a Service (PaaS) Provision</t>
-  </si>
-  <si>
-    <t>Technology provided as a cloud service consisting of managed platform resources</t>
-  </si>
-  <si>
-    <t>SaaSProvision</t>
-  </si>
-  <si>
-    <t>Software as a Service (SaaS) Provision</t>
-  </si>
-  <si>
-    <t>Technology provided as a cloud service consisting of managed software resources</t>
-  </si>
-  <si>
-    <t>CaaSProvision</t>
-  </si>
-  <si>
-    <t>Compute as a Service (CaaS) Provision</t>
-  </si>
-  <si>
-    <t>Technology provided as a cloud service consisting of managed compute resources</t>
-  </si>
-  <si>
-    <t>MBaaSProvision</t>
-  </si>
-  <si>
-    <t>Mobile backend as a Service Provision</t>
-  </si>
-  <si>
-    <t>Technology provided as a cloud service consisting of managed 'backend' services for mobile users</t>
-  </si>
-  <si>
-    <t>ServerlessComputingProvision</t>
-  </si>
-  <si>
-    <t>Serverless Computing Provision</t>
-  </si>
-  <si>
-    <t>Technology provided as a cloud service consisting of fully managed servers for executing functions</t>
-  </si>
-  <si>
-    <t>PrivateCloudServiceProvision</t>
-  </si>
-  <si>
-    <t>Private Cloud Service Provision</t>
-  </si>
-  <si>
-    <t>Technology provided as a cloud service that is private</t>
-  </si>
-  <si>
-    <t>Tek Raj Chhetri</t>
-  </si>
-  <si>
-    <t>PublicCloudServiceProvision</t>
-  </si>
-  <si>
-    <t>Public Cloud Service Provision</t>
-  </si>
-  <si>
-    <t>Technology provided as a cloud service that is public</t>
-  </si>
-  <si>
-    <t>HybridCloudServiceProvision</t>
-  </si>
-  <si>
-    <t>Hybrid Cloud Service Provision</t>
-  </si>
-  <si>
-    <t>Technology provided as a cloud service that is both private and public in parts</t>
-  </si>
-  <si>
-    <t>tech:PrivateCloudService,tech:PublicCloudServiceProvision</t>
-  </si>
-  <si>
-    <t>Proposed for v2.2</t>
-  </si>
-  <si>
-    <t>ConceptStage</t>
-  </si>
-  <si>
-    <t>Concept Stage</t>
-  </si>
-  <si>
-    <t>DevelopmentStage</t>
-  </si>
-  <si>
-    <t>Development Stage</t>
-  </si>
-  <si>
-    <t>ProductionStage</t>
-  </si>
-  <si>
-    <t>Production Stage</t>
-  </si>
-  <si>
-    <t>UtilisationStage</t>
-  </si>
-  <si>
-    <t>Utilisation Stage</t>
-  </si>
-  <si>
-    <t>SupportStage</t>
-  </si>
-  <si>
-    <t>Support Stage</t>
-  </si>
-  <si>
-    <t>RetirementStage</t>
-  </si>
-  <si>
-    <t>Retirement Stage</t>
-  </si>
-  <si>
-    <t>ChangeDescription</t>
-  </si>
-  <si>
-    <t>ChangeStatus</t>
-  </si>
-  <si>
-    <t>ChangeProposed</t>
-  </si>
-  <si>
-    <t>ChangeApproved</t>
-  </si>
-  <si>
-    <t>ChangeRequested</t>
-  </si>
-  <si>
-    <t>ChangeAuthorised</t>
-  </si>
-  <si>
-    <t>ChangeVerified</t>
-  </si>
-  <si>
-    <t>ChangePlanned</t>
-  </si>
-  <si>
-    <t>ChangePending</t>
-  </si>
-  <si>
-    <t>ChangeScheduled</t>
-  </si>
-  <si>
-    <t>ChangeOngoing</t>
-  </si>
-  <si>
-    <t>ChangeCompleted</t>
-  </si>
-  <si>
-    <t>ChangeFailed</t>
-  </si>
-  <si>
-    <t>ChangePaused</t>
-  </si>
-  <si>
-    <t>ChangeReverted</t>
-  </si>
-  <si>
-    <t>ChangeCategory</t>
-  </si>
-  <si>
-    <t>SystematicChangeCategory</t>
-  </si>
-  <si>
-    <t>SystematicChange</t>
-  </si>
-  <si>
-    <t>AdhocChange</t>
-  </si>
-  <si>
-    <t>PlannedChangeCategory</t>
-  </si>
-  <si>
-    <t>PlannedChange</t>
-  </si>
-  <si>
-    <t>Vague broad notion of change planned</t>
-  </si>
-  <si>
-    <t>UnplannedChange</t>
-  </si>
-  <si>
-    <t>Change that is not planned</t>
-  </si>
-  <si>
-    <t>PredeterminedChangeCategory</t>
-  </si>
-  <si>
-    <t>PredeterminedChange</t>
-  </si>
-  <si>
-    <t>Specific determination of change in terms of what to change or when to change - can include reaction to external factors</t>
-  </si>
-  <si>
-    <t>NonpredeterminedChange</t>
-  </si>
-  <si>
-    <t>Change that is not predetermined but is planned</t>
-  </si>
-  <si>
-    <t>IntendedChangeCategory</t>
-  </si>
-  <si>
-    <t>IntendedChange</t>
-  </si>
-  <si>
-    <t>UnintendedChange</t>
-  </si>
-  <si>
-    <t>RateOfChangeCategory</t>
-  </si>
-  <si>
-    <t>GradualChange</t>
-  </si>
-  <si>
-    <t>InstantaneousChange</t>
-  </si>
-  <si>
-    <t>ReversibilityOfChangeCategory</t>
-  </si>
-  <si>
-    <t>ReversibleChange</t>
-  </si>
-  <si>
-    <t>IrreversibleChange</t>
-  </si>
-  <si>
-    <t>TransformationChangeCategory</t>
-  </si>
-  <si>
-    <t>IncrementalChange</t>
-  </si>
-  <si>
-    <t>TransformativeChange</t>
-  </si>
-  <si>
-    <t>ControlOverChangeCategory</t>
-  </si>
-  <si>
-    <t>ControlledChange</t>
-  </si>
-  <si>
-    <t>UncontrolledChange</t>
-  </si>
-  <si>
-    <t>TemporalChangeCategory</t>
-  </si>
-  <si>
-    <t>TemporaryChange</t>
-  </si>
-  <si>
-    <t>LastingChange</t>
-  </si>
-  <si>
-    <t>Actors involved in technologies</t>
-  </si>
-  <si>
-    <t>Provider</t>
-  </si>
-  <si>
-    <t>Actor that provides Technology</t>
-  </si>
-  <si>
-    <t>tech:Actor</t>
-  </si>
-  <si>
-    <t>ISO/IEC 22989:2022</t>
-  </si>
-  <si>
-    <t>Producer</t>
-  </si>
-  <si>
-    <t>Actor that produces Technology</t>
-  </si>
-  <si>
-    <t>Developer</t>
-  </si>
-  <si>
-    <t>Actor that develops Technology</t>
-  </si>
-  <si>
-    <t>tech:Producer</t>
-  </si>
-  <si>
-    <t>Customer</t>
-  </si>
-  <si>
-    <t>Actor that uses Technology directly or indirectly by providing it to Users</t>
-  </si>
-  <si>
-    <t>User</t>
-  </si>
-  <si>
-    <t>Actor that uses Technology</t>
-  </si>
-  <si>
-    <t>tech:Customer</t>
-  </si>
-  <si>
-    <t>Subject</t>
-  </si>
-  <si>
-    <t>Actor that is subjected to the use or impact of Technology</t>
-  </si>
-  <si>
-    <t>Subject can be a human or non-human entity. To explicitly indicate that the subject is a human, and to reuse DPV's human subject taxonomy, the tech:Subject should also be defined as an instance or category of dpv:HumanSubject</t>
-  </si>
-  <si>
-    <t>Deployer</t>
-  </si>
-  <si>
-    <t>Actor that deploys Technology</t>
-  </si>
-  <si>
-    <t>AI Act</t>
-  </si>
-  <si>
-    <t>Designer</t>
-  </si>
-  <si>
-    <t>Actor that designs Technology</t>
-  </si>
-  <si>
-    <t>DGA 26.3</t>
-  </si>
-  <si>
-    <t>Installer</t>
-  </si>
-  <si>
-    <t>Actor that installs Technology</t>
-  </si>
-  <si>
-    <t>Maintainer</t>
-  </si>
-  <si>
-    <t>Actor that maintains Technology</t>
-  </si>
-  <si>
-    <t>Manufacturer</t>
-  </si>
-  <si>
-    <t>Actor that manufactures Technology</t>
-  </si>
-  <si>
-    <t>Owner</t>
-  </si>
-  <si>
-    <t>Actor that owns Technology</t>
-  </si>
-  <si>
-    <t>Purchaser</t>
-  </si>
-  <si>
-    <t>Actor that purchases Technology</t>
-  </si>
-  <si>
-    <t>Supplier</t>
-  </si>
-  <si>
-    <t>Actor that supplies Technology</t>
-  </si>
-  <si>
-    <t>Partner</t>
-  </si>
-  <si>
-    <t>Actor that provides services in the context of Technology</t>
-  </si>
-  <si>
-    <t>"Partner" is a vague term and should not be used - instead the more specific terms provided in this vocabulary should be used. Partner refers to entities that provide services for the technology (as opposed to for using the technology) - for example to further develop or refine it, or to test or audit it.</t>
-  </si>
-  <si>
-    <t>Evaluator</t>
-  </si>
-  <si>
-    <t>Actor that evaluates the performance of Technology</t>
-  </si>
-  <si>
-    <t>tech:Partner</t>
-  </si>
-  <si>
-    <t>Auditor</t>
-  </si>
-  <si>
-    <t>Actor that audits Technology for conformance to policies, standards, or legal requirements</t>
-  </si>
-  <si>
-    <t>SystemIntegrator</t>
-  </si>
-  <si>
-    <t>System Integrator</t>
-  </si>
-  <si>
-    <t>Actor that integrates Technology in to (larger) systems</t>
-  </si>
-  <si>
-    <t>Importer</t>
-  </si>
-  <si>
-    <t>Actor that imports the Technology within a jurisdiction</t>
-  </si>
-  <si>
-    <t>Distributor</t>
-  </si>
-  <si>
-    <t>Actor that distributes the Technology</t>
-  </si>
-  <si>
-    <t>Operator</t>
-  </si>
-  <si>
-    <t>Actor that operates the Technology</t>
-  </si>
-  <si>
-    <t>Operator and User are similar concepts but may refer to different actors, for example in the scenario where the user determines what actions to perform on the technology and the operator executes these actions by operating the technology</t>
-  </si>
-  <si>
-    <t>hasProvider</t>
-  </si>
-  <si>
-    <t>has provider</t>
-  </si>
-  <si>
-    <t>Indicates technology provider</t>
-  </si>
-  <si>
-    <t>tech:Provider</t>
-  </si>
-  <si>
-    <t>tech:hasActor</t>
-  </si>
-  <si>
-    <t>hasProducer</t>
-  </si>
-  <si>
-    <t>has producer</t>
-  </si>
-  <si>
-    <t>Indicates technology producer</t>
-  </si>
-  <si>
-    <t>hasDeveloper</t>
-  </si>
-  <si>
-    <t>has developer</t>
-  </si>
-  <si>
-    <t>Indicates technology developer</t>
-  </si>
-  <si>
-    <t>tech:Developer</t>
-  </si>
-  <si>
-    <t>hasCustomer</t>
-  </si>
-  <si>
-    <t>has customer</t>
-  </si>
-  <si>
-    <t>Indicates technology customer</t>
-  </si>
-  <si>
-    <t>hasUser</t>
-  </si>
-  <si>
-    <t>has user</t>
-  </si>
-  <si>
-    <t>Indicates technology user</t>
-  </si>
-  <si>
-    <t>tech:User</t>
-  </si>
-  <si>
-    <t>hasSubject</t>
-  </si>
-  <si>
-    <t>has subject</t>
-  </si>
-  <si>
-    <t>Indicates technology subject</t>
-  </si>
-  <si>
-    <t>tech:Subject</t>
-  </si>
-  <si>
-    <t>hasDeployer</t>
-  </si>
-  <si>
-    <t>has deployer</t>
-  </si>
-  <si>
-    <t>Indicates technology deployer</t>
-  </si>
-  <si>
-    <t>tech:Deployer</t>
-  </si>
-  <si>
-    <t>hasDesigner</t>
-  </si>
-  <si>
-    <t>has designer</t>
-  </si>
-  <si>
-    <t>Indicates technology designer</t>
-  </si>
-  <si>
-    <t>tech:Designer</t>
-  </si>
-  <si>
-    <t>hasInstaller</t>
-  </si>
-  <si>
-    <t>has installer</t>
-  </si>
-  <si>
-    <t>Indicates technology installer</t>
-  </si>
-  <si>
-    <t>tech:Installer</t>
-  </si>
-  <si>
-    <t>hasMaintainer</t>
-  </si>
-  <si>
-    <t>has maintainer</t>
-  </si>
-  <si>
-    <t>Indicates technology maintainer</t>
-  </si>
-  <si>
-    <t>tech:Maintainer</t>
-  </si>
-  <si>
-    <t>hasManufacturer</t>
-  </si>
-  <si>
-    <t>has manufacturer</t>
-  </si>
-  <si>
-    <t>Indicates technology manufacturer</t>
-  </si>
-  <si>
-    <t>tech:Manufacturer</t>
-  </si>
-  <si>
-    <t>hasOwner</t>
-  </si>
-  <si>
-    <t>has owner</t>
-  </si>
-  <si>
-    <t>Indicates technology owner</t>
-  </si>
-  <si>
-    <t>tech:Owner</t>
-  </si>
-  <si>
-    <t>hasPurchaser</t>
-  </si>
-  <si>
-    <t>has purchaser</t>
-  </si>
-  <si>
-    <t>Indicates technology purchaser</t>
-  </si>
-  <si>
-    <t>tech:Purchaser</t>
-  </si>
-  <si>
-    <t>hasSupplier</t>
-  </si>
-  <si>
-    <t>has supplier</t>
-  </si>
-  <si>
-    <t>Indicates technology supplier</t>
-  </si>
-  <si>
-    <t>tech:Supplier</t>
-  </si>
-  <si>
-    <t>hasPartner</t>
-  </si>
-  <si>
-    <t>has partner</t>
-  </si>
-  <si>
-    <t>Indicates technology partner</t>
-  </si>
-  <si>
-    <t>hasEvaluator</t>
-  </si>
-  <si>
-    <t>has evaluator</t>
-  </si>
-  <si>
-    <t>Indicates technology evaluator</t>
-  </si>
-  <si>
-    <t>tech:Evaluator</t>
-  </si>
-  <si>
-    <t>hasAuditor</t>
-  </si>
-  <si>
-    <t>has auditor</t>
-  </si>
-  <si>
-    <t>Indicates technology auditor</t>
-  </si>
-  <si>
-    <t>tech:Auditor</t>
-  </si>
-  <si>
-    <t>hasSystemIntegrator</t>
-  </si>
-  <si>
-    <t>has system integrator</t>
-  </si>
-  <si>
-    <t>Indicates technology system integrator</t>
-  </si>
-  <si>
-    <t>tech:SystemIntegrator</t>
-  </si>
-  <si>
-    <t>Manual</t>
-  </si>
-  <si>
-    <t>Documentation that provides instructions for using, maintaining, developing, or performing other activities regarding the technology</t>
-  </si>
-  <si>
-    <t>Guide</t>
-  </si>
-  <si>
-    <t>Documentation that provides guidance regarding the technology</t>
-  </si>
-  <si>
-    <t>Instructions</t>
-  </si>
-  <si>
-    <t>Instructions related to technology</t>
-  </si>
-  <si>
-    <t>Specification</t>
-  </si>
-  <si>
-    <t>Documentation that specifies requirements that must be satisfied by the technology</t>
-  </si>
-  <si>
-    <t>Plan</t>
-  </si>
-  <si>
-    <t>Plan associated with using, maintaining, developing, or performing other activities associated with technology</t>
-  </si>
-  <si>
-    <t>TestingPlan</t>
-  </si>
-  <si>
-    <t>Testing Plan</t>
-  </si>
-  <si>
-    <t>Plan associated with testing technology</t>
-  </si>
-  <si>
-    <t>tech:Plan</t>
-  </si>
-  <si>
-    <t>DevelopmentPlan</t>
-  </si>
-  <si>
-    <t>Development Plan</t>
-  </si>
-  <si>
-    <t>Plan associated with developing technology</t>
-  </si>
-  <si>
-    <t>dpv:Status</t>
-  </si>
-  <si>
-    <t>DevelopmentStatus</t>
-  </si>
-  <si>
-    <t>DeploymentStatus</t>
-  </si>
-  <si>
-    <t>TechnologyStatus</t>
-  </si>
-  <si>
-    <t>Technology Status</t>
-  </si>
-  <si>
-    <t>Status associated with development, deployment, and use of technology</t>
-  </si>
-  <si>
-    <t>MarketAvailabilityStatus</t>
-  </si>
-  <si>
-    <t>Market Availability Status</t>
-  </si>
-  <si>
-    <t>Status indicating whether Technology is available on the market</t>
-  </si>
-  <si>
-    <t>tech:TechnologyStatus</t>
-  </si>
-  <si>
-    <t>MarketAvailable</t>
-  </si>
-  <si>
-    <t>Market Available</t>
-  </si>
-  <si>
-    <t>Status indicating Technology is available on the market</t>
-  </si>
-  <si>
-    <t>tech:MarketAvailabilityStatus</t>
-  </si>
-  <si>
-    <t>MarketUnavailable</t>
-  </si>
-  <si>
-    <t>Market Unavailable</t>
-  </si>
-  <si>
-    <t>Status indicating Technology is unavailable on the market</t>
-  </si>
-  <si>
-    <t>ProvisionStatus</t>
-  </si>
-  <si>
-    <t>Provision Status</t>
-  </si>
-  <si>
-    <t>Status indicating whether Technology has been provided</t>
-  </si>
-  <si>
-    <t>Provided</t>
-  </si>
-  <si>
-    <t>Status indicating Technology has been provided</t>
-  </si>
-  <si>
-    <t>tech:ProvisionStatus</t>
-  </si>
-  <si>
-    <t>NotProvided</t>
-  </si>
-  <si>
-    <t>Not Provided</t>
-  </si>
-  <si>
-    <t>Status indicating Technology has not been provided</t>
-  </si>
-  <si>
-    <t>TechnologyReadinessLevel</t>
-  </si>
-  <si>
-    <t>Technology Readiness Level (TRL)</t>
-  </si>
-  <si>
-    <t>Indication of maturity of Technology (ISO 16290:2013)</t>
-  </si>
-  <si>
-    <t>hasTRL</t>
-  </si>
-  <si>
-    <t>has TRL</t>
-  </si>
-  <si>
-    <t>Indicates technology maturity level</t>
-  </si>
-  <si>
-    <t>tech:TechnologyReadinessLevel</t>
-  </si>
-  <si>
-    <t>dpv:hasStatus</t>
-  </si>
-  <si>
-    <t>hasMarketAvailabilityStatus</t>
-  </si>
-  <si>
-    <t>has market availability status</t>
-  </si>
-  <si>
-    <t>Indicates whether the technology is available on the market</t>
-  </si>
-  <si>
-    <t>hasProvisionStatus</t>
-  </si>
-  <si>
-    <t>has provision status</t>
-  </si>
-  <si>
-    <t>Indicates whether the technology has been provided</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>How technology communicates</t>
-  </si>
-  <si>
-    <t>Networking</t>
-  </si>
-  <si>
-    <t>Technology utilising networking</t>
-  </si>
-  <si>
-    <t>LocalNetwork</t>
-  </si>
-  <si>
-    <t>Local Network</t>
-  </si>
-  <si>
-    <t>Technology utilising local networking</t>
-  </si>
-  <si>
-    <t>tech:Networking</t>
-  </si>
-  <si>
-    <t>Internet</t>
-  </si>
-  <si>
-    <t>Technology utilising internet</t>
-  </si>
-  <si>
-    <t>WiFi</t>
-  </si>
-  <si>
-    <t>Technology utilising wifi wireless networking</t>
-  </si>
-  <si>
-    <t>Bluetooth</t>
-  </si>
-  <si>
-    <t>Technology utilising bluetooth</t>
-  </si>
-  <si>
-    <t>CellularNetwork</t>
-  </si>
-  <si>
-    <t>Cellular Network</t>
-  </si>
-  <si>
-    <t>Technology utilising cellular networking</t>
-  </si>
-  <si>
-    <t>GPS</t>
-  </si>
-  <si>
-    <t>Technology utilising GPS</t>
-  </si>
-  <si>
-    <t>Specific instances of technologies</t>
-  </si>
-  <si>
-    <t>Software</t>
-  </si>
-  <si>
-    <t>Virtual parts or components of the technology such as programs and data</t>
-  </si>
-  <si>
-    <t>DataStorage</t>
-  </si>
-  <si>
-    <t>Data Storage</t>
-  </si>
-  <si>
-    <t>Technology associated with storage of data</t>
-  </si>
-  <si>
-    <t>tech:Software</t>
-  </si>
-  <si>
-    <t>Database</t>
-  </si>
-  <si>
-    <t>A database, database management system (DBMS), or application database</t>
-  </si>
-  <si>
-    <t>tech:DataStorage</t>
-  </si>
-  <si>
-    <t>CloudStorage</t>
-  </si>
-  <si>
-    <t>Cloud Storage</t>
-  </si>
-  <si>
-    <t>Storage utilising cloud technologies</t>
-  </si>
-  <si>
-    <t>LocalStorage</t>
-  </si>
-  <si>
-    <t>Local Storage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Storage that is local (e.g. on device) </t>
-  </si>
-  <si>
-    <t>Cookie</t>
-  </si>
-  <si>
-    <t>A HTTP or web or internet cookie</t>
-  </si>
-  <si>
-    <t>tech:LocalStorage</t>
-  </si>
-  <si>
-    <t>Application</t>
-  </si>
-  <si>
-    <t>Application or Application Software</t>
-  </si>
-  <si>
-    <t>SmartphoneApplication</t>
-  </si>
-  <si>
-    <t>Smartphone Application</t>
-  </si>
-  <si>
-    <t>A computing or digital program on a smartphone device</t>
-  </si>
-  <si>
-    <t>tech:Application</t>
-  </si>
-  <si>
-    <t>AppStore</t>
-  </si>
-  <si>
-    <t>Application Store</t>
-  </si>
-  <si>
-    <t>An application or platform for distribution of other applications</t>
-  </si>
-  <si>
-    <t>OS</t>
-  </si>
-  <si>
-    <t>Operating System (OS)</t>
-  </si>
-  <si>
-    <t>Software for managing hardware and other software</t>
-  </si>
-  <si>
-    <t>MSWindows</t>
-  </si>
-  <si>
-    <t>Microsoft Windows</t>
-  </si>
-  <si>
-    <t>Microsoft Windows operating system</t>
-  </si>
-  <si>
-    <t>tech:OS</t>
-  </si>
-  <si>
-    <t>iOS</t>
-  </si>
-  <si>
-    <t>iOS operating system</t>
-  </si>
-  <si>
-    <t>Android</t>
-  </si>
-  <si>
-    <t>Android operating system</t>
-  </si>
-  <si>
-    <t>GNULinux</t>
-  </si>
-  <si>
-    <t>GNU/Linux</t>
-  </si>
-  <si>
-    <t>GNU/Linux operating system</t>
-  </si>
-  <si>
-    <t>Hardware</t>
-  </si>
-  <si>
-    <t>Physical parts or components of the technology</t>
-  </si>
-  <si>
-    <t>Device</t>
-  </si>
-  <si>
-    <t>Device or computing device</t>
-  </si>
-  <si>
-    <t>tech:Hardware</t>
-  </si>
-  <si>
-    <t>PersonalComputer</t>
-  </si>
-  <si>
-    <t>Personal Computer (PC)</t>
-  </si>
-  <si>
-    <t>A computing device intended for individual use</t>
-  </si>
-  <si>
-    <t>tech:Device</t>
-  </si>
-  <si>
-    <t>LaptopPC</t>
-  </si>
-  <si>
-    <t>Laptop PC</t>
-  </si>
-  <si>
-    <t>A portal personal computer</t>
-  </si>
-  <si>
-    <t>tech:PersonalComputer</t>
-  </si>
-  <si>
-    <t>DesktopPC</t>
-  </si>
-  <si>
-    <t>Desktop PC</t>
-  </si>
-  <si>
-    <t>A non-portable or fixed personal computer</t>
-  </si>
-  <si>
-    <t>Telephone</t>
-  </si>
-  <si>
-    <t>MobilePhone</t>
-  </si>
-  <si>
-    <t>Mobile Phone</t>
-  </si>
-  <si>
-    <t>Mobile telephone</t>
-  </si>
-  <si>
-    <t>tech:Telephone</t>
-  </si>
-  <si>
-    <t>Smartphone</t>
-  </si>
-  <si>
-    <t>A combination of a mobile phone with computing capabilities similar to a PC</t>
-  </si>
-  <si>
-    <t>tech:MobilePhone,tech:PersonalComputer</t>
-  </si>
-  <si>
-    <t>IoT</t>
-  </si>
-  <si>
-    <t>Internet of Things (IoT)</t>
-  </si>
-  <si>
-    <t>IoT is the infrastructure of interconnected entities, people, systems and information resources together with services that process and react to information from the physical world and virtual world</t>
-  </si>
-  <si>
-    <t>IoTDevice</t>
-  </si>
-  <si>
-    <t>IoT Device</t>
-  </si>
-  <si>
-    <t>An entity of an IoT system that interacts and communicates with the physical world through sensing or actuating</t>
-  </si>
-  <si>
-    <t>tech:IoT,tech:Device</t>
-  </si>
-  <si>
-    <t>IoTSystem</t>
-  </si>
-  <si>
-    <t>IoT System</t>
-  </si>
-  <si>
-    <t>A specific system that is an implementation or application of the IoT framework and contains interconnected IoT devices and their communication network along with other hardware and software required for providing functionalities</t>
-  </si>
-  <si>
-    <t>tech:IoT,tech:System</t>
-  </si>
-  <si>
-    <t>Model</t>
-  </si>
-  <si>
-    <t>A simplified representation or abstraction of a system, process, or concept</t>
-  </si>
-  <si>
-    <t>Service</t>
-  </si>
-  <si>
-    <t>The carrying out of a specific task or set of tasks as a service</t>
-  </si>
-  <si>
-    <t>This concept is distinct from dpv:Service as it represents the notion of a technical service whereas dpv:Service can also refer to organisational, legal, social, and other meanings of service</t>
-  </si>
-  <si>
-    <t>Algorithm</t>
-  </si>
-  <si>
-    <t>A step-by-step set of instructions used to solve a problem or perform a computation</t>
-  </si>
-  <si>
-    <t>System</t>
-  </si>
-  <si>
-    <t>A collection of components that interact to achieve a specific goal or function</t>
-  </si>
-  <si>
-    <t>Component</t>
-  </si>
-  <si>
-    <t>A self-contained part of a system that performs a specific function and interacts with other components</t>
-  </si>
-  <si>
-    <t>CloudService</t>
-  </si>
-  <si>
-    <t>A remotely accessible service delivered over the internet for providing resources, software, or infrastructure</t>
-  </si>
-  <si>
-    <t>Infrastructure</t>
   </si>
   <si>
     <t>The foundational hardware, software, and other resources to support the operation of systems or services</t>
@@ -6085,10 +6091,10 @@
         <v>596</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>215</v>
+        <v>597</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="D39" s="7"/>
       <c r="E39" s="6" t="s">
@@ -6128,13 +6134,13 @@
     </row>
     <row r="40">
       <c r="A40" s="6" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>219</v>
+        <v>600</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="D40" s="7"/>
       <c r="E40" s="6" t="s">
@@ -6174,16 +6180,16 @@
     </row>
     <row r="41">
       <c r="A41" s="6" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>16</v>
@@ -6222,13 +6228,13 @@
     </row>
     <row r="42">
       <c r="A42" s="6" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="D42" s="7"/>
       <c r="E42" s="6" t="s">
@@ -6268,13 +6274,13 @@
     </row>
     <row r="43">
       <c r="A43" s="6" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>554</v>
@@ -6316,16 +6322,16 @@
     </row>
     <row r="44">
       <c r="A44" s="6" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>16</v>
@@ -6364,13 +6370,13 @@
     </row>
     <row r="45">
       <c r="A45" s="6" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>514</v>
@@ -6412,13 +6418,13 @@
     </row>
     <row r="46">
       <c r="A46" s="6" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>514</v>
@@ -6578,19 +6584,19 @@
     </row>
     <row r="2">
       <c r="A2" s="18" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="D2" s="34" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
@@ -6626,19 +6632,19 @@
     </row>
     <row r="3">
       <c r="A3" s="18" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
@@ -6674,19 +6680,19 @@
     </row>
     <row r="4">
       <c r="A4" s="18" t="s">
+        <v>625</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>626</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>627</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>624</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>623</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>624</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>625</v>
-      </c>
-      <c r="D4" s="34" t="s">
-        <v>622</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>621</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -6722,19 +6728,19 @@
     </row>
     <row r="5">
       <c r="A5" s="18" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -6770,19 +6776,19 @@
     </row>
     <row r="6">
       <c r="A6" s="18" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c r="D6" s="34" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -6818,13 +6824,13 @@
     </row>
     <row r="7">
       <c r="A7" s="18" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>16</v>
@@ -6833,7 +6839,7 @@
         <v>558</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -6868,13 +6874,13 @@
     </row>
     <row r="8">
       <c r="A8" s="18" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>16</v>
@@ -6916,13 +6922,13 @@
     </row>
     <row r="9">
       <c r="A9" s="18" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>16</v>
@@ -6964,13 +6970,13 @@
     </row>
     <row r="10">
       <c r="A10" s="18" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>16</v>
@@ -7012,19 +7018,19 @@
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="K11" s="19">
         <v>45627.0</v>
@@ -7039,19 +7045,19 @@
     </row>
     <row r="12">
       <c r="A12" s="18" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
@@ -7087,19 +7093,19 @@
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
@@ -7135,19 +7141,19 @@
     </row>
     <row r="14">
       <c r="A14" s="6" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
@@ -7321,27 +7327,27 @@
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="B2" s="5"/>
       <c r="J2" s="10" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
     </row>
     <row r="6">
@@ -7836,26 +7842,26 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>16</v>
@@ -7865,7 +7871,7 @@
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N3" s="6" t="s">
         <v>39</v>
@@ -7876,16 +7882,16 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
+        <v>676</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>677</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>678</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>674</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>675</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>676</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>672</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>16</v>
@@ -7895,7 +7901,7 @@
       </c>
       <c r="L4" s="8"/>
       <c r="M4" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N4" s="6" t="s">
         <v>39</v>
@@ -7906,16 +7912,16 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>16</v>
@@ -7925,7 +7931,7 @@
       </c>
       <c r="L5" s="8"/>
       <c r="M5" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N5" s="6" t="s">
         <v>39</v>
@@ -7936,16 +7942,16 @@
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>16</v>
@@ -7955,7 +7961,7 @@
       </c>
       <c r="L6" s="8"/>
       <c r="M6" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N6" s="6" t="s">
         <v>39</v>
@@ -7966,16 +7972,16 @@
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>16</v>
@@ -7985,7 +7991,7 @@
       </c>
       <c r="L7" s="8"/>
       <c r="M7" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N7" s="6" t="s">
         <v>39</v>
@@ -7996,16 +8002,16 @@
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>16</v>
@@ -8015,7 +8021,7 @@
       </c>
       <c r="L8" s="8"/>
       <c r="M8" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N8" s="6" t="s">
         <v>39</v>
@@ -8026,16 +8032,16 @@
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>16</v>
@@ -8045,7 +8051,7 @@
       </c>
       <c r="L9" s="8"/>
       <c r="M9" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N9" s="6" t="s">
         <v>39</v>
@@ -8056,16 +8062,16 @@
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>16</v>
@@ -8075,7 +8081,7 @@
       </c>
       <c r="L10" s="8"/>
       <c r="M10" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N10" s="6" t="s">
         <v>39</v>
@@ -8086,16 +8092,16 @@
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>16</v>
@@ -8105,7 +8111,7 @@
       </c>
       <c r="L11" s="8"/>
       <c r="M11" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N11" s="6" t="s">
         <v>39</v>
@@ -8116,16 +8122,16 @@
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>16</v>
@@ -8135,7 +8141,7 @@
       </c>
       <c r="L12" s="8"/>
       <c r="M12" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N12" s="6" t="s">
         <v>39</v>
@@ -8146,16 +8152,16 @@
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>16</v>
@@ -8164,7 +8170,7 @@
         <v>44727.0</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N13" s="6" t="s">
         <v>39</v>
@@ -8175,16 +8181,16 @@
     </row>
     <row r="14">
       <c r="A14" s="24" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="C14" s="48" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="D14" s="49" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>16</v>
@@ -8194,12 +8200,12 @@
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
       <c r="J14" s="24" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="K14" s="11"/>
       <c r="L14" s="11"/>
       <c r="M14" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N14" s="11"/>
       <c r="O14" s="11"/>
@@ -8222,18 +8228,18 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>16</v>
@@ -8242,7 +8248,7 @@
         <v>44727.0</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N17" s="6" t="s">
         <v>39</v>
@@ -8253,13 +8259,13 @@
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>16</v>
@@ -8269,7 +8275,7 @@
       </c>
       <c r="L18" s="8"/>
       <c r="M18" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N18" s="6" t="s">
         <v>39</v>
@@ -8280,13 +8286,13 @@
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>16</v>
@@ -8296,7 +8302,7 @@
       </c>
       <c r="L19" s="8"/>
       <c r="M19" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N19" s="6" t="s">
         <v>39</v>
@@ -8307,13 +8313,13 @@
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>16</v>
@@ -8323,7 +8329,7 @@
       </c>
       <c r="L20" s="8"/>
       <c r="M20" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N20" s="6" t="s">
         <v>39</v>
@@ -8334,13 +8340,13 @@
     </row>
     <row r="21">
       <c r="A21" s="6" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>16</v>
@@ -8350,7 +8356,7 @@
       </c>
       <c r="L21" s="8"/>
       <c r="M21" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N21" s="6" t="s">
         <v>39</v>
@@ -8361,13 +8367,13 @@
     </row>
     <row r="22">
       <c r="A22" s="6" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>16</v>
@@ -8377,7 +8383,7 @@
       </c>
       <c r="L22" s="8"/>
       <c r="M22" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N22" s="6" t="s">
         <v>39</v>
@@ -8388,10 +8394,10 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="30"/>
@@ -8400,16 +8406,16 @@
     </row>
     <row r="25">
       <c r="A25" s="6" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>16</v>
@@ -8418,7 +8424,7 @@
         <v>44727.0</v>
       </c>
       <c r="M25" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N25" s="6" t="s">
         <v>39</v>
@@ -8429,16 +8435,16 @@
     </row>
     <row r="26">
       <c r="A26" s="6" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="B26" s="6" t="s">
+        <v>737</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>738</v>
+      </c>
+      <c r="D26" s="30" t="s">
         <v>735</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>736</v>
-      </c>
-      <c r="D26" s="30" t="s">
-        <v>733</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>16</v>
@@ -8447,7 +8453,7 @@
         <v>44727.0</v>
       </c>
       <c r="M26" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N26" s="6" t="s">
         <v>39</v>
@@ -8458,16 +8464,16 @@
     </row>
     <row r="27">
       <c r="A27" s="6" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>16</v>
@@ -8476,7 +8482,7 @@
         <v>44727.0</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N27" s="6" t="s">
         <v>39</v>
@@ -8493,10 +8499,10 @@
         <v>527</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>16</v>
@@ -8505,7 +8511,7 @@
         <v>44727.0</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N28" s="6" t="s">
         <v>39</v>
@@ -8516,10 +8522,10 @@
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -8550,16 +8556,16 @@
     </row>
     <row r="31">
       <c r="A31" s="6" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>16</v>
@@ -8568,10 +8574,10 @@
         <v>44727.0</v>
       </c>
       <c r="M31" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N31" s="6" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="O31" s="9" t="s">
         <v>28</v>
@@ -8579,16 +8585,16 @@
     </row>
     <row r="32">
       <c r="A32" s="6" t="s">
+        <v>749</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>751</v>
+      </c>
+      <c r="D32" s="6" t="s">
         <v>747</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>748</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>749</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>745</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>16</v>
@@ -8597,10 +8603,10 @@
         <v>44727.0</v>
       </c>
       <c r="M32" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N32" s="6" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="O32" s="9" t="s">
         <v>28</v>
@@ -8608,16 +8614,16 @@
     </row>
     <row r="33">
       <c r="A33" s="6" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>16</v>
@@ -8626,10 +8632,10 @@
         <v>44727.0</v>
       </c>
       <c r="M33" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="O33" s="9" t="s">
         <v>28</v>
@@ -8637,16 +8643,16 @@
     </row>
     <row r="34">
       <c r="A34" s="6" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>16</v>
@@ -8655,10 +8661,10 @@
         <v>44727.0</v>
       </c>
       <c r="M34" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N34" s="6" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="O34" s="9" t="s">
         <v>28</v>
@@ -8666,16 +8672,16 @@
     </row>
     <row r="35">
       <c r="A35" s="6" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>16</v>
@@ -8684,10 +8690,10 @@
         <v>44727.0</v>
       </c>
       <c r="M35" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N35" s="6" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="O35" s="9" t="s">
         <v>28</v>
@@ -8695,16 +8701,16 @@
     </row>
     <row r="36">
       <c r="A36" s="6" t="s">
-        <v>759</v>
+        <v>761</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>760</v>
+        <v>762</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>16</v>
@@ -8713,10 +8719,10 @@
         <v>44727.0</v>
       </c>
       <c r="M36" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N36" s="6" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="O36" s="9" t="s">
         <v>28</v>
@@ -8724,37 +8730,37 @@
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="K38" s="8"/>
     </row>
     <row r="39">
       <c r="A39" s="6" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>16</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>768</v>
+        <v>770</v>
       </c>
       <c r="K39" s="8">
         <v>44727.0</v>
       </c>
       <c r="M39" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N39" s="6" t="s">
         <v>39</v>
@@ -8765,28 +8771,28 @@
     </row>
     <row r="40">
       <c r="A40" s="6" t="s">
+        <v>771</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>772</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>773</v>
+      </c>
+      <c r="D40" s="6" t="s">
         <v>769</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>770</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>771</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>767</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>16</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
       <c r="K40" s="8">
         <v>44727.0</v>
       </c>
       <c r="M40" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N40" s="6" t="s">
         <v>39</v>
@@ -8797,21 +8803,21 @@
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="32" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
       <c r="C43" s="32" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c r="D43" s="35" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>16</v>
@@ -8820,7 +8826,7 @@
         <v>44727.0</v>
       </c>
       <c r="M43" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N43" s="6" t="s">
         <v>39</v>
@@ -8831,16 +8837,16 @@
     </row>
     <row r="44">
       <c r="A44" s="50" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="B44" s="50" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="C44" s="51" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="D44" s="52" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="E44" s="11" t="s">
         <v>16</v>
@@ -8855,7 +8861,7 @@
       </c>
       <c r="L44" s="11"/>
       <c r="M44" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N44" s="11" t="s">
         <v>39</v>
@@ -8881,16 +8887,16 @@
     </row>
     <row r="45">
       <c r="A45" s="50" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="B45" s="50" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="C45" s="51" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="D45" s="55" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="E45" s="11" t="s">
         <v>16</v>
@@ -8905,7 +8911,7 @@
       </c>
       <c r="L45" s="11"/>
       <c r="M45" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N45" s="11" t="s">
         <v>39</v>
@@ -8931,16 +8937,16 @@
     </row>
     <row r="46">
       <c r="A46" s="50" t="s">
-        <v>786</v>
+        <v>788</v>
       </c>
       <c r="B46" s="50" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
       <c r="C46" s="51" t="s">
-        <v>788</v>
+        <v>790</v>
       </c>
       <c r="D46" s="55" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="E46" s="11" t="s">
         <v>16</v>
@@ -8955,7 +8961,7 @@
       </c>
       <c r="L46" s="11"/>
       <c r="M46" s="6" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="N46" s="11" t="s">
         <v>39</v>
@@ -11396,7 +11402,6 @@
       <c r="AB11" s="7"/>
     </row>
     <row r="12">
-      <c r="A12" s="6"/>
       <c r="L12" s="8"/>
     </row>
     <row r="13">

</xml_diff>

<commit_message>
Adds Location concepts to TECH ; #342
- Marks concepts in TECH tools module as locations
- Adds broader parent types based on `dpv:ProcessingLocation` and
  `dpv:StorageLocation`, as well as `dpv:LocalLocation` for local
  storage technologies
- Has RDF, and in HTML also provides a note on usage

Co-authored-by: Julian Flake <flake@uni-koblenz.de>
</commit_message>
<xml_diff>
--- a/code/vocab_csv/tech.xlsx
+++ b/code/vocab_csv/tech.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1888" uniqueCount="820">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1896" uniqueCount="833">
   <si>
     <t>Term</t>
   </si>
@@ -1608,6 +1608,9 @@
     <t>Technology utilising GPS</t>
   </si>
   <si>
+    <t>This concept models GPS as a networking technology. For representing use of GPS to get current location, see pd:GPSCoordinate and pd:CurrentLocation concepts in PD extension</t>
+  </si>
+  <si>
     <t>Specific instances of technologies</t>
   </si>
   <si>
@@ -1626,81 +1629,99 @@
     <t>Technology associated with storage of data</t>
   </si>
   <si>
+    <t>tech:Software,dpv:StorageLocation,dpv:ProcessingLocation</t>
+  </si>
+  <si>
+    <t>dpv:Technology,dpv:Location</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>A database, database management system (DBMS), or application database</t>
+  </si>
+  <si>
+    <t>tech:DataStorage,dpv:StorageLocation,dpv:ProcessingLocation</t>
+  </si>
+  <si>
+    <t>CloudStorage</t>
+  </si>
+  <si>
+    <t>Cloud Storage</t>
+  </si>
+  <si>
+    <t>Storage utilising cloud technologies</t>
+  </si>
+  <si>
+    <t>tech:DataStorage,dpv:StorageLocation,dpv:ProcessingLocation,dpv:CloudLocation</t>
+  </si>
+  <si>
+    <t>LocalStorage</t>
+  </si>
+  <si>
+    <t>Local Storage</t>
+  </si>
+  <si>
+    <t>Storage that is local (e.g. on device)</t>
+  </si>
+  <si>
+    <t>tech:DataStorage,dpv:ProcessingLocation,dpv:LocalLocation</t>
+  </si>
+  <si>
+    <t>Cookie</t>
+  </si>
+  <si>
+    <t>A HTTP or web or internet cookie</t>
+  </si>
+  <si>
+    <t>tech:LocalStorage,dpv:ProcessingLocation,dpv:LocalLocation</t>
+  </si>
+  <si>
+    <t>Application</t>
+  </si>
+  <si>
+    <t>Application or Application Software</t>
+  </si>
+  <si>
+    <t>tech:Software,dpv:ProcessingLocation,dpv:LocalLocation</t>
+  </si>
+  <si>
+    <t>SmartphoneApplication</t>
+  </si>
+  <si>
+    <t>Smartphone Application</t>
+  </si>
+  <si>
+    <t>A computing or digital program on a smartphone device</t>
+  </si>
+  <si>
+    <t>tech:Application,dpv:ProcessingLocation,dpv:LocalLocation</t>
+  </si>
+  <si>
+    <t>AppStore</t>
+  </si>
+  <si>
+    <t>Application Store</t>
+  </si>
+  <si>
+    <t>An application or platform for distribution of other applications</t>
+  </si>
+  <si>
+    <t>tech:Application</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>Operating System (OS)</t>
+  </si>
+  <si>
+    <t>Software for managing hardware and other software</t>
+  </si>
+  <si>
     <t>tech:Software</t>
   </si>
   <si>
-    <t>Database</t>
-  </si>
-  <si>
-    <t>A database, database management system (DBMS), or application database</t>
-  </si>
-  <si>
-    <t>tech:DataStorage</t>
-  </si>
-  <si>
-    <t>CloudStorage</t>
-  </si>
-  <si>
-    <t>Cloud Storage</t>
-  </si>
-  <si>
-    <t>Storage utilising cloud technologies</t>
-  </si>
-  <si>
-    <t>LocalStorage</t>
-  </si>
-  <si>
-    <t>Local Storage</t>
-  </si>
-  <si>
-    <t>Storage that is local (e.g. on device)</t>
-  </si>
-  <si>
-    <t>Cookie</t>
-  </si>
-  <si>
-    <t>A HTTP or web or internet cookie</t>
-  </si>
-  <si>
-    <t>tech:LocalStorage</t>
-  </si>
-  <si>
-    <t>Application</t>
-  </si>
-  <si>
-    <t>Application or Application Software</t>
-  </si>
-  <si>
-    <t>SmartphoneApplication</t>
-  </si>
-  <si>
-    <t>Smartphone Application</t>
-  </si>
-  <si>
-    <t>A computing or digital program on a smartphone device</t>
-  </si>
-  <si>
-    <t>tech:Application</t>
-  </si>
-  <si>
-    <t>AppStore</t>
-  </si>
-  <si>
-    <t>Application Store</t>
-  </si>
-  <si>
-    <t>An application or platform for distribution of other applications</t>
-  </si>
-  <si>
-    <t>OS</t>
-  </si>
-  <si>
-    <t>Operating System (OS)</t>
-  </si>
-  <si>
-    <t>Software for managing hardware and other software</t>
-  </si>
-  <si>
     <t>MSWindows</t>
   </si>
   <si>
@@ -1746,171 +1767,177 @@
     <t>Device or computing device</t>
   </si>
   <si>
+    <t>tech:Hardware,dpv:ProcessingLocation,dpv:LocalLocation</t>
+  </si>
+  <si>
+    <t>PersonalComputer</t>
+  </si>
+  <si>
+    <t>Personal Computer (PC)</t>
+  </si>
+  <si>
+    <t>A computing device intended for individual use</t>
+  </si>
+  <si>
+    <t>tech:Device,dpv:ProcessingLocation,dpv:LocalLocation</t>
+  </si>
+  <si>
+    <t>LaptopPC</t>
+  </si>
+  <si>
+    <t>Laptop PC</t>
+  </si>
+  <si>
+    <t>A portal personal computer</t>
+  </si>
+  <si>
+    <t>tech:PersonalComputer,dpv:ProcessingLocation,dpv:LocalLocation</t>
+  </si>
+  <si>
+    <t>DesktopPC</t>
+  </si>
+  <si>
+    <t>Desktop PC</t>
+  </si>
+  <si>
+    <t>A non-portable or fixed personal computer</t>
+  </si>
+  <si>
+    <t>Telephone</t>
+  </si>
+  <si>
+    <t>tech:Device</t>
+  </si>
+  <si>
+    <t>MobilePhone</t>
+  </si>
+  <si>
+    <t>Mobile Phone</t>
+  </si>
+  <si>
+    <t>Mobile telephone</t>
+  </si>
+  <si>
+    <t>tech:Telephone,dpv:ProcessingLocation,dpv:LocalLocation</t>
+  </si>
+  <si>
+    <t>Smartphone</t>
+  </si>
+  <si>
+    <t>A combination of a mobile phone with computing capabilities similar to a PC</t>
+  </si>
+  <si>
+    <t>tech:MobilePhone,tech:PersonalComputer,dpv:ProcessingLocation,dpv:LocalLocation</t>
+  </si>
+  <si>
+    <t>IoT</t>
+  </si>
+  <si>
+    <t>Internet of Things (IoT)</t>
+  </si>
+  <si>
+    <t>IoT is the infrastructure of interconnected entities, people, systems and information resources together with services that process and react to information from the physical world and virtual world</t>
+  </si>
+  <si>
+    <t>IoTDevice</t>
+  </si>
+  <si>
+    <t>IoT Device</t>
+  </si>
+  <si>
+    <t>An entity of an IoT system that interacts and communicates with the physical world through sensing or actuating</t>
+  </si>
+  <si>
+    <t>tech:IoT,tech:Device,dpv:ProcessingLocation,dpv:LocalLocation</t>
+  </si>
+  <si>
+    <t>IoTSystem</t>
+  </si>
+  <si>
+    <t>IoT System</t>
+  </si>
+  <si>
+    <t>A specific system that is an implementation or application of the IoT framework and contains interconnected IoT devices and their communication network along with other hardware and software required for providing functionalities</t>
+  </si>
+  <si>
+    <t>tech:IoT,tech:System,dpv:ProcessingLocation,dpv:LocalLocation</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>A simplified representation or abstraction of a system, process, or concept</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>The carrying out of a specific task or set of tasks as a service</t>
+  </si>
+  <si>
+    <t>This concept is distinct from dpv:Service as it represents the notion of a technical service whereas dpv:Service can also refer to organisational, legal, social, and other meanings of service</t>
+  </si>
+  <si>
+    <t>Algorithm</t>
+  </si>
+  <si>
+    <t>A step-by-step set of instructions used to solve a problem or perform a computation</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+  <si>
+    <t>A collection of components that interact to achieve a specific goal or function</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>A self-contained part of a system that performs a specific function and interacts with other components</t>
+  </si>
+  <si>
+    <t>CloudService</t>
+  </si>
+  <si>
+    <t>Cloud Service Provision</t>
+  </si>
+  <si>
+    <t>A remotely accessible service delivered over the internet for providing resources, software, or infrastructure</t>
+  </si>
+  <si>
+    <t>Infrastructure</t>
+  </si>
+  <si>
+    <t>Infrastructure as a Service (IaaS) Provision</t>
+  </si>
+  <si>
+    <t>The foundational hardware, software, and other resources to support the operation of systems or services</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>A set of rules and protocols to communicate and exchange data between applications</t>
+  </si>
+  <si>
+    <t>tech:Algorithm</t>
+  </si>
+  <si>
+    <t>Platform</t>
+  </si>
+  <si>
+    <t>A digital environment that provides tools, infrastructure, and services for developing, deploying, and running applications</t>
+  </si>
+  <si>
+    <t>IntegratedCircuit</t>
+  </si>
+  <si>
+    <t>A integrated electronic chip containing interconnected components to perform specific functions</t>
+  </si>
+  <si>
     <t>tech:Hardware</t>
   </si>
   <si>
-    <t>PersonalComputer</t>
-  </si>
-  <si>
-    <t>Personal Computer (PC)</t>
-  </si>
-  <si>
-    <t>A computing device intended for individual use</t>
-  </si>
-  <si>
-    <t>tech:Device</t>
-  </si>
-  <si>
-    <t>LaptopPC</t>
-  </si>
-  <si>
-    <t>Laptop PC</t>
-  </si>
-  <si>
-    <t>A portal personal computer</t>
-  </si>
-  <si>
-    <t>tech:PersonalComputer</t>
-  </si>
-  <si>
-    <t>DesktopPC</t>
-  </si>
-  <si>
-    <t>Desktop PC</t>
-  </si>
-  <si>
-    <t>A non-portable or fixed personal computer</t>
-  </si>
-  <si>
-    <t>Telephone</t>
-  </si>
-  <si>
-    <t>MobilePhone</t>
-  </si>
-  <si>
-    <t>Mobile Phone</t>
-  </si>
-  <si>
-    <t>Mobile telephone</t>
-  </si>
-  <si>
-    <t>tech:Telephone</t>
-  </si>
-  <si>
-    <t>Smartphone</t>
-  </si>
-  <si>
-    <t>A combination of a mobile phone with computing capabilities similar to a PC</t>
-  </si>
-  <si>
-    <t>tech:MobilePhone,tech:PersonalComputer</t>
-  </si>
-  <si>
-    <t>IoT</t>
-  </si>
-  <si>
-    <t>Internet of Things (IoT)</t>
-  </si>
-  <si>
-    <t>IoT is the infrastructure of interconnected entities, people, systems and information resources together with services that process and react to information from the physical world and virtual world</t>
-  </si>
-  <si>
-    <t>IoTDevice</t>
-  </si>
-  <si>
-    <t>IoT Device</t>
-  </si>
-  <si>
-    <t>An entity of an IoT system that interacts and communicates with the physical world through sensing or actuating</t>
-  </si>
-  <si>
-    <t>tech:IoT,tech:Device</t>
-  </si>
-  <si>
-    <t>IoTSystem</t>
-  </si>
-  <si>
-    <t>IoT System</t>
-  </si>
-  <si>
-    <t>A specific system that is an implementation or application of the IoT framework and contains interconnected IoT devices and their communication network along with other hardware and software required for providing functionalities</t>
-  </si>
-  <si>
-    <t>tech:IoT,tech:System</t>
-  </si>
-  <si>
-    <t>Model</t>
-  </si>
-  <si>
-    <t>A simplified representation or abstraction of a system, process, or concept</t>
-  </si>
-  <si>
-    <t>Service</t>
-  </si>
-  <si>
-    <t>The carrying out of a specific task or set of tasks as a service</t>
-  </si>
-  <si>
-    <t>This concept is distinct from dpv:Service as it represents the notion of a technical service whereas dpv:Service can also refer to organisational, legal, social, and other meanings of service</t>
-  </si>
-  <si>
-    <t>Algorithm</t>
-  </si>
-  <si>
-    <t>A step-by-step set of instructions used to solve a problem or perform a computation</t>
-  </si>
-  <si>
-    <t>System</t>
-  </si>
-  <si>
-    <t>A collection of components that interact to achieve a specific goal or function</t>
-  </si>
-  <si>
-    <t>Component</t>
-  </si>
-  <si>
-    <t>A self-contained part of a system that performs a specific function and interacts with other components</t>
-  </si>
-  <si>
-    <t>CloudService</t>
-  </si>
-  <si>
-    <t>Cloud Service Provision</t>
-  </si>
-  <si>
-    <t>A remotely accessible service delivered over the internet for providing resources, software, or infrastructure</t>
-  </si>
-  <si>
-    <t>Infrastructure</t>
-  </si>
-  <si>
-    <t>Infrastructure as a Service (IaaS) Provision</t>
-  </si>
-  <si>
-    <t>The foundational hardware, software, and other resources to support the operation of systems or services</t>
-  </si>
-  <si>
-    <t>API</t>
-  </si>
-  <si>
-    <t>A set of rules and protocols to communicate and exchange data between applications</t>
-  </si>
-  <si>
-    <t>tech:Algorithm</t>
-  </si>
-  <si>
-    <t>Platform</t>
-  </si>
-  <si>
-    <t>A digital environment that provides tools, infrastructure, and services for developing, deploying, and running applications</t>
-  </si>
-  <si>
-    <t>IntegratedCircuit</t>
-  </si>
-  <si>
-    <t>A integrated electronic chip containing interconnected components to perform specific functions</t>
-  </si>
-  <si>
     <t>ApplicationSpecificIntegratedCircuit</t>
   </si>
   <si>
@@ -1957,6 +1984,18 @@
   </si>
   <si>
     <t>User Agent as defined here specifically represents software agents that represent humans, whether directly or indirectly, based on the well-defined use of this term in Web interactions. Software that is not representing a human but which acts or declares itself as a user agent is termed as 'user agent spoofing' (see https://developer.mozilla.org/en-US/docs/Glossary/User_agent)</t>
+  </si>
+  <si>
+    <t>WebScraper</t>
+  </si>
+  <si>
+    <t>Web Scraper</t>
+  </si>
+  <si>
+    <t>Software that extracts data from websites to implement collection practices colloquially called "web scraping"</t>
+  </si>
+  <si>
+    <t>Delaram Golpayegani</t>
   </si>
   <si>
     <t>hasSystem</t>
@@ -4667,7 +4706,9 @@
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
+      <c r="I10" s="6" t="s">
+        <v>527</v>
+      </c>
       <c r="J10" s="7"/>
       <c r="K10" s="8">
         <v>45421.0</v>
@@ -4796,10 +4837,10 @@
     </row>
     <row r="2">
       <c r="A2" s="31" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="C2" s="32"/>
       <c r="D2" s="33"/>
@@ -4818,13 +4859,13 @@
     </row>
     <row r="4">
       <c r="A4" s="31" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="D4" s="34"/>
       <c r="E4" s="6" t="s">
@@ -4874,19 +4915,19 @@
     </row>
     <row r="6">
       <c r="A6" s="31" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>16</v>
+        <v>535</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -4922,19 +4963,19 @@
     </row>
     <row r="7">
       <c r="A7" s="32" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="C7" s="32" t="s">
+        <v>537</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>538</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>535</v>
-      </c>
-      <c r="D7" s="35" t="s">
-        <v>536</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>16</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -4972,19 +5013,19 @@
     </row>
     <row r="8">
       <c r="A8" s="18" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="D8" s="35" t="s">
-        <v>536</v>
+        <v>542</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>16</v>
+        <v>535</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
@@ -5020,19 +5061,19 @@
     </row>
     <row r="9">
       <c r="A9" s="18" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>536</v>
+        <v>546</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>16</v>
+        <v>535</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
@@ -5068,19 +5109,19 @@
     </row>
     <row r="10">
       <c r="A10" s="32" t="s">
-        <v>543</v>
+        <v>547</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>543</v>
+        <v>547</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>544</v>
+        <v>548</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>16</v>
+        <v>535</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
@@ -5118,19 +5159,19 @@
     </row>
     <row r="12">
       <c r="A12" s="31" t="s">
-        <v>546</v>
+        <v>550</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>546</v>
+        <v>550</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>547</v>
+        <v>551</v>
       </c>
       <c r="D12" s="35" t="s">
-        <v>533</v>
+        <v>552</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>16</v>
+        <v>535</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
@@ -5166,19 +5207,19 @@
     </row>
     <row r="13">
       <c r="A13" s="32" t="s">
-        <v>548</v>
+        <v>553</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>549</v>
+        <v>554</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>550</v>
+        <v>555</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>551</v>
+        <v>556</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>16</v>
+        <v>535</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
@@ -5216,16 +5257,16 @@
     </row>
     <row r="14">
       <c r="A14" s="6" t="s">
-        <v>552</v>
+        <v>557</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>553</v>
+        <v>558</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>554</v>
+        <v>559</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>16</v>
@@ -5264,16 +5305,16 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>555</v>
+        <v>561</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>556</v>
+        <v>562</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>557</v>
+        <v>563</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>533</v>
+        <v>564</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>16</v>
@@ -5312,16 +5353,16 @@
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>558</v>
+        <v>565</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>559</v>
+        <v>566</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>560</v>
+        <v>567</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>561</v>
+        <v>568</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>16</v>
@@ -5360,16 +5401,16 @@
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>562</v>
+        <v>569</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>562</v>
+        <v>569</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>563</v>
+        <v>570</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>561</v>
+        <v>568</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>16</v>
@@ -5408,16 +5449,16 @@
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>564</v>
+        <v>571</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>564</v>
+        <v>571</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>565</v>
+        <v>572</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>561</v>
+        <v>568</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>16</v>
@@ -5456,16 +5497,16 @@
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>566</v>
+        <v>573</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>567</v>
+        <v>574</v>
       </c>
       <c r="C20" s="6" t="s">
+        <v>575</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>568</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>561</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>16</v>
@@ -5504,13 +5545,13 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>569</v>
+        <v>576</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>569</v>
+        <v>576</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>570</v>
+        <v>577</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="6" t="s">
@@ -5553,19 +5594,19 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>571</v>
+        <v>578</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>571</v>
+        <v>578</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>572</v>
+        <v>579</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>573</v>
+        <v>580</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>16</v>
+        <v>535</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
@@ -5601,19 +5642,19 @@
     </row>
     <row r="25">
       <c r="A25" s="6" t="s">
-        <v>574</v>
+        <v>581</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>575</v>
+        <v>582</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>576</v>
+        <v>583</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>577</v>
+        <v>584</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>16</v>
+        <v>535</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
@@ -5649,19 +5690,19 @@
     </row>
     <row r="26">
       <c r="A26" s="6" t="s">
-        <v>578</v>
+        <v>585</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>579</v>
+        <v>586</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>580</v>
+        <v>587</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>581</v>
+        <v>588</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>16</v>
+        <v>535</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
@@ -5697,19 +5738,19 @@
     </row>
     <row r="27">
       <c r="A27" s="6" t="s">
-        <v>582</v>
+        <v>589</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>583</v>
+        <v>590</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>584</v>
+        <v>591</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>581</v>
+        <v>588</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>16</v>
+        <v>535</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
@@ -5745,16 +5786,16 @@
     </row>
     <row r="28">
       <c r="A28" s="6" t="s">
-        <v>585</v>
+        <v>592</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>585</v>
+        <v>592</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>585</v>
+        <v>592</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>577</v>
+        <v>593</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>16</v>
@@ -5793,19 +5834,19 @@
     </row>
     <row r="29">
       <c r="A29" s="6" t="s">
-        <v>586</v>
+        <v>594</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>587</v>
+        <v>595</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>588</v>
+        <v>596</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>589</v>
+        <v>597</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>16</v>
+        <v>535</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
@@ -5841,19 +5882,19 @@
     </row>
     <row r="30">
       <c r="A30" s="6" t="s">
-        <v>590</v>
+        <v>598</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>590</v>
+        <v>598</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>591</v>
+        <v>599</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>592</v>
+        <v>600</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>16</v>
+        <v>535</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
@@ -5889,19 +5930,19 @@
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>593</v>
+        <v>601</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>594</v>
+        <v>602</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>573</v>
+        <v>580</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>16</v>
+        <v>535</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
@@ -5939,19 +5980,19 @@
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>596</v>
+        <v>604</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>597</v>
+        <v>605</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>598</v>
+        <v>606</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>599</v>
+        <v>607</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>16</v>
+        <v>535</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
@@ -5989,19 +6030,19 @@
     </row>
     <row r="33">
       <c r="A33" s="6" t="s">
-        <v>600</v>
+        <v>608</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>601</v>
+        <v>609</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>602</v>
+        <v>610</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>16</v>
+        <v>535</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
@@ -6039,13 +6080,13 @@
     </row>
     <row r="34">
       <c r="A34" s="6" t="s">
-        <v>604</v>
+        <v>612</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>604</v>
+        <v>612</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>605</v>
+        <v>613</v>
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="6" t="s">
@@ -6085,13 +6126,13 @@
     </row>
     <row r="35">
       <c r="A35" s="6" t="s">
-        <v>606</v>
+        <v>614</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>606</v>
+        <v>614</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>607</v>
+        <v>615</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="6" t="s">
@@ -6101,7 +6142,7 @@
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
       <c r="I35" s="6" t="s">
-        <v>608</v>
+        <v>616</v>
       </c>
       <c r="J35" s="7"/>
       <c r="K35" s="19">
@@ -6133,13 +6174,13 @@
     </row>
     <row r="36">
       <c r="A36" s="6" t="s">
-        <v>609</v>
+        <v>617</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>609</v>
+        <v>617</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>610</v>
+        <v>618</v>
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="6" t="s">
@@ -6179,13 +6220,13 @@
     </row>
     <row r="37">
       <c r="A37" s="6" t="s">
-        <v>611</v>
+        <v>619</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>611</v>
+        <v>619</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>612</v>
+        <v>620</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="6" t="s">
@@ -6225,13 +6266,13 @@
     </row>
     <row r="38">
       <c r="A38" s="6" t="s">
-        <v>613</v>
+        <v>621</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>613</v>
+        <v>621</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>614</v>
+        <v>622</v>
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="6" t="s">
@@ -6271,13 +6312,13 @@
     </row>
     <row r="39">
       <c r="A39" s="6" t="s">
-        <v>615</v>
+        <v>623</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>616</v>
+        <v>624</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>617</v>
+        <v>625</v>
       </c>
       <c r="D39" s="7"/>
       <c r="E39" s="6" t="s">
@@ -6317,13 +6358,13 @@
     </row>
     <row r="40">
       <c r="A40" s="6" t="s">
-        <v>618</v>
+        <v>626</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>619</v>
+        <v>627</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>620</v>
+        <v>628</v>
       </c>
       <c r="D40" s="7"/>
       <c r="E40" s="6" t="s">
@@ -6363,16 +6404,16 @@
     </row>
     <row r="41">
       <c r="A41" s="6" t="s">
-        <v>621</v>
+        <v>629</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>621</v>
+        <v>629</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>622</v>
+        <v>630</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>623</v>
+        <v>631</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>16</v>
@@ -6411,13 +6452,13 @@
     </row>
     <row r="42">
       <c r="A42" s="6" t="s">
-        <v>624</v>
+        <v>632</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>624</v>
+        <v>632</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>625</v>
+        <v>633</v>
       </c>
       <c r="D42" s="7"/>
       <c r="E42" s="6" t="s">
@@ -6457,16 +6498,16 @@
     </row>
     <row r="43">
       <c r="A43" s="6" t="s">
-        <v>626</v>
+        <v>634</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>626</v>
+        <v>634</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>627</v>
+        <v>635</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>573</v>
+        <v>636</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>16</v>
@@ -6505,16 +6546,16 @@
     </row>
     <row r="44">
       <c r="A44" s="6" t="s">
-        <v>628</v>
+        <v>637</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>628</v>
+        <v>637</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>629</v>
+        <v>638</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>630</v>
+        <v>639</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>16</v>
@@ -6553,16 +6594,16 @@
     </row>
     <row r="45">
       <c r="A45" s="6" t="s">
-        <v>631</v>
+        <v>640</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>631</v>
+        <v>640</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>632</v>
+        <v>641</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>533</v>
+        <v>564</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>16</v>
@@ -6601,16 +6642,16 @@
     </row>
     <row r="46">
       <c r="A46" s="6" t="s">
-        <v>633</v>
+        <v>642</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>633</v>
+        <v>642</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>634</v>
+        <v>643</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>533</v>
+        <v>564</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>16</v>
@@ -6649,16 +6690,16 @@
     </row>
     <row r="48">
       <c r="A48" s="6" t="s">
-        <v>635</v>
+        <v>644</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>636</v>
+        <v>645</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>637</v>
+        <v>646</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>16</v>
@@ -6697,16 +6738,16 @@
     </row>
     <row r="49">
       <c r="A49" s="6" t="s">
-        <v>639</v>
+        <v>648</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>640</v>
+        <v>649</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>641</v>
+        <v>650</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>642</v>
+        <v>651</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>16</v>
@@ -6715,7 +6756,7 @@
       <c r="G49" s="7"/>
       <c r="H49" s="7"/>
       <c r="I49" s="6" t="s">
-        <v>643</v>
+        <v>652</v>
       </c>
       <c r="J49" s="7"/>
       <c r="K49" s="8">
@@ -6744,6 +6785,54 @@
       <c r="AB49" s="7"/>
       <c r="AC49" s="7"/>
       <c r="AD49" s="7"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="6" t="s">
+        <v>653</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>564</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="7"/>
+      <c r="I51" s="7"/>
+      <c r="J51" s="7"/>
+      <c r="K51" s="8">
+        <v>46062.0</v>
+      </c>
+      <c r="L51" s="7"/>
+      <c r="M51" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="N51" s="6" t="s">
+        <v>656</v>
+      </c>
+      <c r="O51" s="7"/>
+      <c r="P51" s="7"/>
+      <c r="Q51" s="7"/>
+      <c r="R51" s="7"/>
+      <c r="S51" s="7"/>
+      <c r="T51" s="7"/>
+      <c r="U51" s="7"/>
+      <c r="V51" s="7"/>
+      <c r="W51" s="7"/>
+      <c r="X51" s="7"/>
+      <c r="Y51" s="7"/>
+      <c r="Z51" s="7"/>
+      <c r="AA51" s="7"/>
+      <c r="AB51" s="7"/>
+      <c r="AC51" s="7"/>
+      <c r="AD51" s="7"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B39:B40">
@@ -6865,19 +6954,19 @@
     </row>
     <row r="2">
       <c r="A2" s="18" t="s">
-        <v>644</v>
+        <v>657</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>645</v>
+        <v>658</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>646</v>
+        <v>659</v>
       </c>
       <c r="D2" s="34" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>647</v>
+        <v>660</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
@@ -6913,19 +7002,19 @@
     </row>
     <row r="3">
       <c r="A3" s="18" t="s">
-        <v>648</v>
+        <v>661</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>649</v>
+        <v>662</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>650</v>
+        <v>663</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>651</v>
+        <v>664</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>652</v>
+        <v>665</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
@@ -6961,19 +7050,19 @@
     </row>
     <row r="4">
       <c r="A4" s="18" t="s">
-        <v>653</v>
+        <v>666</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>654</v>
+        <v>667</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>655</v>
+        <v>668</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>652</v>
+        <v>665</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>651</v>
+        <v>664</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -7009,19 +7098,19 @@
     </row>
     <row r="5">
       <c r="A5" s="18" t="s">
-        <v>656</v>
+        <v>669</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>657</v>
+        <v>670</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>658</v>
+        <v>671</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>623</v>
+        <v>631</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -7057,19 +7146,19 @@
     </row>
     <row r="6">
       <c r="A6" s="18" t="s">
-        <v>659</v>
+        <v>672</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>660</v>
+        <v>673</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>661</v>
+        <v>674</v>
       </c>
       <c r="D6" s="34" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>662</v>
+        <v>675</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -7105,22 +7194,22 @@
     </row>
     <row r="7">
       <c r="A7" s="18" t="s">
-        <v>663</v>
+        <v>676</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>664</v>
+        <v>677</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>665</v>
+        <v>678</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>577</v>
+        <v>593</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>666</v>
+        <v>679</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -7155,19 +7244,19 @@
     </row>
     <row r="8">
       <c r="A8" s="18" t="s">
-        <v>667</v>
+        <v>680</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>668</v>
+        <v>681</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>669</v>
+        <v>682</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>533</v>
+        <v>564</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
@@ -7203,19 +7292,19 @@
     </row>
     <row r="9">
       <c r="A9" s="18" t="s">
-        <v>670</v>
+        <v>683</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>671</v>
+        <v>684</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>672</v>
+        <v>685</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>573</v>
+        <v>636</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
@@ -7251,19 +7340,19 @@
     </row>
     <row r="10">
       <c r="A10" s="18" t="s">
-        <v>673</v>
+        <v>686</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>674</v>
+        <v>687</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>675</v>
+        <v>688</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
@@ -7299,19 +7388,19 @@
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
-        <v>676</v>
+        <v>689</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>677</v>
+        <v>690</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>678</v>
+        <v>691</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>679</v>
+        <v>692</v>
       </c>
       <c r="K11" s="19">
         <v>45627.0</v>
@@ -7326,19 +7415,19 @@
     </row>
     <row r="12">
       <c r="A12" s="18" t="s">
-        <v>680</v>
+        <v>693</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>681</v>
+        <v>694</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>682</v>
+        <v>695</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>683</v>
+        <v>696</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
@@ -7374,19 +7463,19 @@
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>684</v>
+        <v>697</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>685</v>
+        <v>698</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>686</v>
+        <v>699</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>687</v>
+        <v>700</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
@@ -7422,19 +7511,19 @@
     </row>
     <row r="14">
       <c r="A14" s="6" t="s">
-        <v>688</v>
+        <v>701</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>689</v>
+        <v>702</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>690</v>
+        <v>703</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>691</v>
+        <v>704</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
@@ -7608,27 +7697,27 @@
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>692</v>
+        <v>705</v>
       </c>
       <c r="B2" s="5"/>
       <c r="J2" s="10" t="s">
-        <v>693</v>
+        <v>706</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>694</v>
+        <v>707</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>695</v>
+        <v>708</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>696</v>
+        <v>709</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>697</v>
+        <v>710</v>
       </c>
     </row>
     <row r="6">
@@ -8123,26 +8212,26 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>698</v>
+        <v>711</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>698</v>
+        <v>711</v>
       </c>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>699</v>
+        <v>712</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>700</v>
+        <v>713</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>701</v>
+        <v>714</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>702</v>
+        <v>715</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>16</v>
@@ -8152,7 +8241,7 @@
       </c>
       <c r="L3" s="8"/>
       <c r="M3" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N3" s="6" t="s">
         <v>39</v>
@@ -8163,16 +8252,16 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>704</v>
+        <v>717</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>705</v>
+        <v>718</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>706</v>
+        <v>719</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>702</v>
+        <v>715</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>16</v>
@@ -8182,7 +8271,7 @@
       </c>
       <c r="L4" s="8"/>
       <c r="M4" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N4" s="6" t="s">
         <v>39</v>
@@ -8193,16 +8282,16 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>707</v>
+        <v>720</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>708</v>
+        <v>721</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>709</v>
+        <v>722</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>702</v>
+        <v>715</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>16</v>
@@ -8212,7 +8301,7 @@
       </c>
       <c r="L5" s="8"/>
       <c r="M5" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N5" s="6" t="s">
         <v>39</v>
@@ -8223,16 +8312,16 @@
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>710</v>
+        <v>723</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>711</v>
+        <v>724</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>712</v>
+        <v>725</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>702</v>
+        <v>715</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>16</v>
@@ -8242,7 +8331,7 @@
       </c>
       <c r="L6" s="8"/>
       <c r="M6" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N6" s="6" t="s">
         <v>39</v>
@@ -8253,16 +8342,16 @@
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>713</v>
+        <v>726</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>714</v>
+        <v>727</v>
       </c>
       <c r="C7" s="6" t="s">
+        <v>728</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>715</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>702</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>16</v>
@@ -8272,7 +8361,7 @@
       </c>
       <c r="L7" s="8"/>
       <c r="M7" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N7" s="6" t="s">
         <v>39</v>
@@ -8283,16 +8372,16 @@
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
-        <v>716</v>
+        <v>729</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>717</v>
+        <v>730</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>718</v>
+        <v>731</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>702</v>
+        <v>715</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>16</v>
@@ -8302,7 +8391,7 @@
       </c>
       <c r="L8" s="8"/>
       <c r="M8" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N8" s="6" t="s">
         <v>39</v>
@@ -8313,16 +8402,16 @@
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>719</v>
+        <v>732</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>720</v>
+        <v>733</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>721</v>
+        <v>734</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>702</v>
+        <v>715</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>16</v>
@@ -8332,7 +8421,7 @@
       </c>
       <c r="L9" s="8"/>
       <c r="M9" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N9" s="6" t="s">
         <v>39</v>
@@ -8343,16 +8432,16 @@
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
-        <v>722</v>
+        <v>735</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>723</v>
+        <v>736</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>724</v>
+        <v>737</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>702</v>
+        <v>715</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>16</v>
@@ -8362,7 +8451,7 @@
       </c>
       <c r="L10" s="8"/>
       <c r="M10" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N10" s="6" t="s">
         <v>39</v>
@@ -8373,16 +8462,16 @@
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
-        <v>725</v>
+        <v>738</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>726</v>
+        <v>739</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>727</v>
+        <v>740</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>702</v>
+        <v>715</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>16</v>
@@ -8392,7 +8481,7 @@
       </c>
       <c r="L11" s="8"/>
       <c r="M11" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N11" s="6" t="s">
         <v>39</v>
@@ -8403,16 +8492,16 @@
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>728</v>
+        <v>741</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>729</v>
+        <v>742</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>730</v>
+        <v>743</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>731</v>
+        <v>744</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>16</v>
@@ -8422,7 +8511,7 @@
       </c>
       <c r="L12" s="8"/>
       <c r="M12" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N12" s="6" t="s">
         <v>39</v>
@@ -8433,16 +8522,16 @@
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>732</v>
+        <v>745</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>733</v>
+        <v>746</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>734</v>
+        <v>747</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>735</v>
+        <v>748</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>16</v>
@@ -8451,7 +8540,7 @@
         <v>44727.0</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N13" s="6" t="s">
         <v>39</v>
@@ -8462,16 +8551,16 @@
     </row>
     <row r="14">
       <c r="A14" s="24" t="s">
-        <v>736</v>
+        <v>749</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>737</v>
+        <v>750</v>
       </c>
       <c r="C14" s="48" t="s">
-        <v>738</v>
+        <v>751</v>
       </c>
       <c r="D14" s="49" t="s">
-        <v>702</v>
+        <v>715</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>16</v>
@@ -8481,12 +8570,12 @@
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
       <c r="J14" s="24" t="s">
-        <v>739</v>
+        <v>752</v>
       </c>
       <c r="K14" s="11"/>
       <c r="L14" s="11"/>
       <c r="M14" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N14" s="11"/>
       <c r="O14" s="11"/>
@@ -8509,18 +8598,18 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>740</v>
+        <v>753</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>741</v>
+        <v>754</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>742</v>
+        <v>755</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>743</v>
+        <v>756</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>16</v>
@@ -8529,7 +8618,7 @@
         <v>44727.0</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N17" s="6" t="s">
         <v>39</v>
@@ -8540,13 +8629,13 @@
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>744</v>
+        <v>757</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>745</v>
+        <v>758</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>746</v>
+        <v>759</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>16</v>
@@ -8556,7 +8645,7 @@
       </c>
       <c r="L18" s="8"/>
       <c r="M18" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N18" s="6" t="s">
         <v>39</v>
@@ -8567,13 +8656,13 @@
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>747</v>
+        <v>760</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>748</v>
+        <v>761</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>749</v>
+        <v>762</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>16</v>
@@ -8583,7 +8672,7 @@
       </c>
       <c r="L19" s="8"/>
       <c r="M19" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N19" s="6" t="s">
         <v>39</v>
@@ -8594,13 +8683,13 @@
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>750</v>
+        <v>763</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>751</v>
+        <v>764</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>752</v>
+        <v>765</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>16</v>
@@ -8610,7 +8699,7 @@
       </c>
       <c r="L20" s="8"/>
       <c r="M20" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N20" s="6" t="s">
         <v>39</v>
@@ -8621,13 +8710,13 @@
     </row>
     <row r="21">
       <c r="A21" s="6" t="s">
-        <v>753</v>
+        <v>766</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>754</v>
+        <v>767</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>755</v>
+        <v>768</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>16</v>
@@ -8637,7 +8726,7 @@
       </c>
       <c r="L21" s="8"/>
       <c r="M21" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N21" s="6" t="s">
         <v>39</v>
@@ -8648,13 +8737,13 @@
     </row>
     <row r="22">
       <c r="A22" s="6" t="s">
-        <v>756</v>
+        <v>769</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>757</v>
+        <v>770</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>758</v>
+        <v>771</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>16</v>
@@ -8664,7 +8753,7 @@
       </c>
       <c r="L22" s="8"/>
       <c r="M22" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N22" s="6" t="s">
         <v>39</v>
@@ -8675,10 +8764,10 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>759</v>
+        <v>772</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>759</v>
+        <v>772</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="30"/>
@@ -8687,16 +8776,16 @@
     </row>
     <row r="25">
       <c r="A25" s="6" t="s">
-        <v>760</v>
+        <v>773</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>761</v>
+        <v>774</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>762</v>
+        <v>775</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>763</v>
+        <v>776</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>16</v>
@@ -8705,7 +8794,7 @@
         <v>44727.0</v>
       </c>
       <c r="M25" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N25" s="6" t="s">
         <v>39</v>
@@ -8716,16 +8805,16 @@
     </row>
     <row r="26">
       <c r="A26" s="6" t="s">
-        <v>764</v>
+        <v>777</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>765</v>
+        <v>778</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>766</v>
+        <v>779</v>
       </c>
       <c r="D26" s="30" t="s">
-        <v>763</v>
+        <v>776</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>16</v>
@@ -8734,7 +8823,7 @@
         <v>44727.0</v>
       </c>
       <c r="M26" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N26" s="6" t="s">
         <v>39</v>
@@ -8745,16 +8834,16 @@
     </row>
     <row r="27">
       <c r="A27" s="6" t="s">
-        <v>767</v>
+        <v>780</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>768</v>
+        <v>781</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>769</v>
+        <v>782</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>763</v>
+        <v>776</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>16</v>
@@ -8763,7 +8852,7 @@
         <v>44727.0</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N27" s="6" t="s">
         <v>39</v>
@@ -8774,16 +8863,16 @@
     </row>
     <row r="28">
       <c r="A28" s="6" t="s">
-        <v>546</v>
+        <v>550</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>546</v>
+        <v>550</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>770</v>
+        <v>783</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>763</v>
+        <v>776</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>16</v>
@@ -8792,7 +8881,7 @@
         <v>44727.0</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N28" s="6" t="s">
         <v>39</v>
@@ -8803,10 +8892,10 @@
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>771</v>
+        <v>784</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>771</v>
+        <v>784</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -8837,16 +8926,16 @@
     </row>
     <row r="31">
       <c r="A31" s="6" t="s">
-        <v>772</v>
+        <v>785</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>773</v>
+        <v>786</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>774</v>
+        <v>787</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>775</v>
+        <v>788</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>16</v>
@@ -8855,10 +8944,10 @@
         <v>44727.0</v>
       </c>
       <c r="M31" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N31" s="6" t="s">
-        <v>776</v>
+        <v>789</v>
       </c>
       <c r="O31" s="9" t="s">
         <v>28</v>
@@ -8866,16 +8955,16 @@
     </row>
     <row r="32">
       <c r="A32" s="6" t="s">
-        <v>777</v>
+        <v>790</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>778</v>
+        <v>791</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>779</v>
+        <v>792</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>775</v>
+        <v>788</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>16</v>
@@ -8884,10 +8973,10 @@
         <v>44727.0</v>
       </c>
       <c r="M32" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N32" s="6" t="s">
-        <v>776</v>
+        <v>789</v>
       </c>
       <c r="O32" s="9" t="s">
         <v>28</v>
@@ -8895,16 +8984,16 @@
     </row>
     <row r="33">
       <c r="A33" s="6" t="s">
-        <v>780</v>
+        <v>793</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>781</v>
+        <v>794</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>782</v>
+        <v>795</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>775</v>
+        <v>788</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>16</v>
@@ -8913,10 +9002,10 @@
         <v>44727.0</v>
       </c>
       <c r="M33" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>776</v>
+        <v>789</v>
       </c>
       <c r="O33" s="9" t="s">
         <v>28</v>
@@ -8924,16 +9013,16 @@
     </row>
     <row r="34">
       <c r="A34" s="6" t="s">
-        <v>783</v>
+        <v>796</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>784</v>
+        <v>797</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>785</v>
+        <v>798</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>775</v>
+        <v>788</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>16</v>
@@ -8942,10 +9031,10 @@
         <v>44727.0</v>
       </c>
       <c r="M34" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N34" s="6" t="s">
-        <v>776</v>
+        <v>789</v>
       </c>
       <c r="O34" s="9" t="s">
         <v>28</v>
@@ -8953,16 +9042,16 @@
     </row>
     <row r="35">
       <c r="A35" s="6" t="s">
-        <v>786</v>
+        <v>799</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>787</v>
+        <v>800</v>
       </c>
       <c r="C35" s="6" t="s">
+        <v>801</v>
+      </c>
+      <c r="D35" s="6" t="s">
         <v>788</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>775</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>16</v>
@@ -8971,10 +9060,10 @@
         <v>44727.0</v>
       </c>
       <c r="M35" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N35" s="6" t="s">
-        <v>776</v>
+        <v>789</v>
       </c>
       <c r="O35" s="9" t="s">
         <v>28</v>
@@ -8982,16 +9071,16 @@
     </row>
     <row r="36">
       <c r="A36" s="6" t="s">
-        <v>789</v>
+        <v>802</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>790</v>
+        <v>803</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>791</v>
+        <v>804</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>792</v>
+        <v>805</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>16</v>
@@ -9000,10 +9089,10 @@
         <v>44727.0</v>
       </c>
       <c r="M36" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N36" s="6" t="s">
-        <v>776</v>
+        <v>789</v>
       </c>
       <c r="O36" s="9" t="s">
         <v>28</v>
@@ -9011,37 +9100,37 @@
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>793</v>
+        <v>806</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>793</v>
+        <v>806</v>
       </c>
       <c r="K38" s="8"/>
     </row>
     <row r="39">
       <c r="A39" s="6" t="s">
-        <v>794</v>
+        <v>807</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>795</v>
+        <v>808</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>796</v>
+        <v>809</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>797</v>
+        <v>810</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>16</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>798</v>
+        <v>811</v>
       </c>
       <c r="K39" s="8">
         <v>44727.0</v>
       </c>
       <c r="M39" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N39" s="6" t="s">
         <v>39</v>
@@ -9052,28 +9141,28 @@
     </row>
     <row r="40">
       <c r="A40" s="6" t="s">
-        <v>799</v>
+        <v>812</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>800</v>
+        <v>813</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>801</v>
+        <v>814</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>797</v>
+        <v>810</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>16</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>802</v>
+        <v>815</v>
       </c>
       <c r="K40" s="8">
         <v>44727.0</v>
       </c>
       <c r="M40" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N40" s="6" t="s">
         <v>39</v>
@@ -9084,21 +9173,21 @@
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>803</v>
+        <v>816</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="32" t="s">
-        <v>804</v>
+        <v>817</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>805</v>
+        <v>818</v>
       </c>
       <c r="C43" s="32" t="s">
-        <v>806</v>
+        <v>819</v>
       </c>
       <c r="D43" s="35" t="s">
-        <v>807</v>
+        <v>820</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>16</v>
@@ -9107,7 +9196,7 @@
         <v>44727.0</v>
       </c>
       <c r="M43" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N43" s="6" t="s">
         <v>39</v>
@@ -9118,16 +9207,16 @@
     </row>
     <row r="44">
       <c r="A44" s="50" t="s">
-        <v>808</v>
+        <v>821</v>
       </c>
       <c r="B44" s="50" t="s">
-        <v>809</v>
+        <v>822</v>
       </c>
       <c r="C44" s="51" t="s">
-        <v>810</v>
+        <v>823</v>
       </c>
       <c r="D44" s="52" t="s">
-        <v>811</v>
+        <v>824</v>
       </c>
       <c r="E44" s="11" t="s">
         <v>16</v>
@@ -9142,7 +9231,7 @@
       </c>
       <c r="L44" s="11"/>
       <c r="M44" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N44" s="11" t="s">
         <v>39</v>
@@ -9168,16 +9257,16 @@
     </row>
     <row r="45">
       <c r="A45" s="50" t="s">
-        <v>812</v>
+        <v>825</v>
       </c>
       <c r="B45" s="50" t="s">
-        <v>813</v>
+        <v>826</v>
       </c>
       <c r="C45" s="51" t="s">
-        <v>814</v>
+        <v>827</v>
       </c>
       <c r="D45" s="55" t="s">
-        <v>815</v>
+        <v>828</v>
       </c>
       <c r="E45" s="11" t="s">
         <v>16</v>
@@ -9192,7 +9281,7 @@
       </c>
       <c r="L45" s="11"/>
       <c r="M45" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N45" s="11" t="s">
         <v>39</v>
@@ -9218,16 +9307,16 @@
     </row>
     <row r="46">
       <c r="A46" s="50" t="s">
-        <v>816</v>
+        <v>829</v>
       </c>
       <c r="B46" s="50" t="s">
-        <v>817</v>
+        <v>830</v>
       </c>
       <c r="C46" s="56" t="s">
-        <v>818</v>
+        <v>831</v>
       </c>
       <c r="D46" s="55" t="s">
-        <v>819</v>
+        <v>832</v>
       </c>
       <c r="E46" s="11" t="s">
         <v>16</v>
@@ -9242,7 +9331,7 @@
       </c>
       <c r="L46" s="11"/>
       <c r="M46" s="6" t="s">
-        <v>703</v>
+        <v>716</v>
       </c>
       <c r="N46" s="11" t="s">
         <v>39</v>

</xml_diff>